<commit_message>
Update VRAM patch stride table.xlsx
</commit_message>
<xml_diff>
--- a/VRAM patch stride table.xlsx
+++ b/VRAM patch stride table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAADFFD-CAA5-45B5-977C-447CA21A8AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D1EA39-7EE9-4DDF-8704-70AA46901756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="28680" yWindow="2505" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>VRAM usage GB</t>
   </si>
@@ -50,28 +50,43 @@
     <t>patch x</t>
   </si>
   <si>
-    <t>stride z</t>
-  </si>
-  <si>
-    <t>stride y</t>
-  </si>
-  <si>
-    <t>stride x</t>
-  </si>
-  <si>
     <t>(resolution)</t>
   </si>
   <si>
-    <t>VRAM per image</t>
-  </si>
-  <si>
-    <t>n train images</t>
-  </si>
-  <si>
     <t>run</t>
   </si>
   <si>
     <t>230818-0?</t>
+  </si>
+  <si>
+    <t>n images</t>
+  </si>
+  <si>
+    <t>n patches</t>
+  </si>
+  <si>
+    <t>VRAM/image</t>
+  </si>
+  <si>
+    <t>VRAM/patch</t>
+  </si>
+  <si>
+    <t>(stride z)</t>
+  </si>
+  <si>
+    <t>(stride y)</t>
+  </si>
+  <si>
+    <t>(stride x)</t>
+  </si>
+  <si>
+    <t>n raw channels</t>
+  </si>
+  <si>
+    <t>pixels/patch/channel</t>
+  </si>
+  <si>
+    <t>pixels/specimen_raw</t>
   </si>
 </sst>
 </file>
@@ -116,11 +131,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,84 +451,121 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="8.85546875"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
-      </c>
-      <c r="R1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
       </c>
       <c r="B2">
         <v>33</v>
       </c>
-      <c r="C2" s="2">
-        <v>3</v>
+      <c r="C2">
+        <v>5</v>
       </c>
       <c r="D2">
         <f>B2/C2</f>
-        <v>11</v>
+        <v>6.6</v>
       </c>
       <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <f>B2/E2</f>
+        <v>6.6</v>
+      </c>
+      <c r="G2" s="1">
         <v>105</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>1140</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>394</v>
       </c>
-      <c r="H2" s="1">
+      <c r="J2">
+        <f>G2*H2*I2</f>
+        <v>47161800</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <f>J2*K2</f>
+        <v>141485400</v>
+      </c>
+      <c r="O2" s="1">
         <v>10</v>
       </c>
-      <c r="I2" s="3">
+      <c r="P2">
         <v>10</v>
       </c>
-      <c r="J2" s="3">
+      <c r="Q2">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
determine valid patch and stride shapes. get some VRAM prediction data
</commit_message>
<xml_diff>
--- a/VRAM patch stride table.xlsx
+++ b/VRAM patch stride table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D1EA39-7EE9-4DDF-8704-70AA46901756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7A13D2-90D4-4875-A3A5-7AE9AD08A3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2505" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>VRAM usage GB</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
   <si>
     <t>patch z</t>
   </si>
@@ -50,15 +47,6 @@
     <t>patch x</t>
   </si>
   <si>
-    <t>(resolution)</t>
-  </si>
-  <si>
-    <t>run</t>
-  </si>
-  <si>
-    <t>230818-0?</t>
-  </si>
-  <si>
     <t>n images</t>
   </si>
   <si>
@@ -87,16 +75,208 @@
   </si>
   <si>
     <t>pixels/specimen_raw</t>
+  </si>
+  <si>
+    <t>230901-0</t>
+  </si>
+  <si>
+    <t>230901-1</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>stride = resolution - patch</t>
+  </si>
+  <si>
+    <t>stride = (resolution - patch) + 1</t>
+  </si>
+  <si>
+    <t>res. Z</t>
+  </si>
+  <si>
+    <t>res. Y</t>
+  </si>
+  <si>
+    <t>res. X</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>AssertionError: datasets should not be an empty iterable</t>
+  </si>
+  <si>
+    <t>stride = (resolution - patch) / 2</t>
+  </si>
+  <si>
+    <t>230901-2</t>
+  </si>
+  <si>
+    <t>230901-3</t>
+  </si>
+  <si>
+    <t>230901-4</t>
+  </si>
+  <si>
+    <t>230901-5</t>
+  </si>
+  <si>
+    <t>230901-6</t>
+  </si>
+  <si>
+    <t>torch.cuda.OutOfMemoryError: CUDA out of memory. Tried to allocate 1.20 GiB (GPU 0; 31.74 GiB total capacity; 29.37 GiB already allocated; 1.06 GiB free; 29.47 GiB reserved in total by PyTorch) If reserved memory is &gt;&gt; allocated memory try setting max_split_size_mb to avoid fragmentation.  See documentation for Memory Management and PYTORCH_CUDA_ALLOC_CONF</t>
+  </si>
+  <si>
+    <t>comments to stride</t>
+  </si>
+  <si>
+    <t>comments to patch</t>
+  </si>
+  <si>
+    <t>patch = (resolution - arbitrary_value)</t>
+  </si>
+  <si>
+    <t>ValueError: requested an output size of torch.Size([9, 38, 116]), but valid sizes range from [7, 37, 115] to [8, 38, 116] (for an input of torch.Size([4, 19, 58]))</t>
+  </si>
+  <si>
+    <t>file of error origin</t>
+  </si>
+  <si>
+    <t>output padding, assignment of 'output_padding'</t>
+  </si>
+  <si>
+    <t>patch = an arbitrary even int_2^3</t>
+  </si>
+  <si>
+    <t>patch = an arbitrary int_2^3 (odd, even mixed)</t>
+  </si>
+  <si>
+    <t>stride = (resolution - patch) / 2, round down to largest int_2^3 (odd, even mixed)</t>
+  </si>
+  <si>
+    <t>stride = (resolution - patch) / 2, round down to largest odd int_2^3</t>
+  </si>
+  <si>
+    <t>torch.cuda.OutOfMemoryError: CUDA out of memory. Tried to allocate 70.00 MiB (GPU 0; 31.74 GiB total capacity; 30.43 GiB already allocated; 11.12 MiB free; 30.53 GiB reserved in total by PyTorch) If reserved memory is &gt;&gt; allocated memory try setting max_split_size_mb to avoid fragmentation.  See documentation for Memory Management and PYTORCH_CUDA_ALLOC_CONF</t>
+  </si>
+  <si>
+    <t>230901-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  File "/home/dwalth/data/conda/envs/3dunet/lib/python3.11/site-packages/torch/nn/functional.py", line 3165, in binary_cross_entropy_with_logits
+    return torch.binary_cross_entropy_with_logits(input, target, weight, pos_weight, reduction_enum)</t>
+  </si>
+  <si>
+    <t>Tesla V100-SXM2-32GB</t>
+  </si>
+  <si>
+    <t>&gt;32768</t>
+  </si>
+  <si>
+    <t>patch = an arbitrary odd int_2^3</t>
+  </si>
+  <si>
+    <t>230901-8</t>
+  </si>
+  <si>
+    <t>session</t>
+  </si>
+  <si>
+    <t>VRAM capacity (MiB)</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>VRAM usage (MiB)</t>
+  </si>
+  <si>
+    <t>ValueError: requested an output size of torch.Size([9, 21, 51]), but valid sizes range from [7, 19, 49] to [8, 20, 50] (for an input of torch.Size([4, 10, 25]))</t>
+  </si>
+  <si>
+    <t>Are odd int_2^3 in patch valid? (with odd int_2^3 stride)</t>
+  </si>
+  <si>
+    <t>Are odd int_2^3 in patch valid? (with even int_2^3 stride)</t>
+  </si>
+  <si>
+    <t>Are even int_2^3 in patch valid? (with odd int_2^3 stride)</t>
+  </si>
+  <si>
+    <t>Are even int_2^3 in patch valid? (with even int_2^3 stride)</t>
+  </si>
+  <si>
+    <t>230901-9</t>
+  </si>
+  <si>
+    <t>230901-10</t>
+  </si>
+  <si>
+    <t>230901-11</t>
+  </si>
+  <si>
+    <t>stride = (resolution - patch) / 2, round down to largest even int_2^3</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>230901-12</t>
+  </si>
+  <si>
+    <t>230901-13</t>
+  </si>
+  <si>
+    <t>230901-14</t>
+  </si>
+  <si>
+    <t>train patch = val patch</t>
+  </si>
+  <si>
+    <t>train stride = val stride</t>
+  </si>
+  <si>
+    <t>reduce VRAM usage</t>
+  </si>
+  <si>
+    <t>230830-0</t>
+  </si>
+  <si>
+    <t>result/answer</t>
+  </si>
+  <si>
+    <t>goal/question</t>
+  </si>
+  <si>
+    <t>better performance metrics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,7 +290,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -127,13 +307,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,128 +644,1087 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875"/>
+    <col min="9" max="9" width="12.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="12.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="5.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.140625" customWidth="1"/>
+    <col min="13" max="13" width="5" customWidth="1"/>
+    <col min="14" max="14" width="6.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" customWidth="1"/>
+    <col min="16" max="17" width="5" customWidth="1"/>
+    <col min="18" max="18" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6" customWidth="1"/>
+    <col min="22" max="22" width="44" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="76.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="142" customWidth="1"/>
+    <col min="25" max="25" width="142" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="O1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="AD1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>33</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <f>B2/C2</f>
-        <v>6.6</v>
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
       </c>
       <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <f>B2/E2</f>
-        <v>6.6</v>
-      </c>
-      <c r="G2" s="1">
+        <v>32768</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2" t="e">
+        <f>D2/G2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J2" t="e">
+        <f>D2/H2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K2" s="1">
         <v>105</v>
       </c>
-      <c r="H2">
-        <v>1140</v>
-      </c>
-      <c r="I2">
+      <c r="L2">
+        <v>1149</v>
+      </c>
+      <c r="M2">
         <v>394</v>
       </c>
-      <c r="J2">
-        <f>G2*H2*I2</f>
-        <v>47161800</v>
-      </c>
-      <c r="K2">
-        <v>3</v>
-      </c>
-      <c r="L2">
-        <f>J2*K2</f>
-        <v>141485400</v>
-      </c>
-      <c r="O2" s="1">
+      <c r="N2" s="1">
+        <v>10</v>
+      </c>
+      <c r="O2">
         <v>10</v>
       </c>
       <c r="P2">
         <v>10</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" s="1">
+        <v>125</v>
+      </c>
+      <c r="S2">
+        <v>1169</v>
+      </c>
+      <c r="T2">
+        <v>414</v>
+      </c>
+      <c r="U2" t="s">
+        <v>61</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB2">
+        <f>K2*L2*M2</f>
+        <v>47534130</v>
+      </c>
+      <c r="AC2">
+        <v>3</v>
+      </c>
+      <c r="AD2">
+        <f>AB2*AC2</f>
+        <v>142602390</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <v>32768</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
         <v>10</v>
+      </c>
+      <c r="I3" t="e">
+        <f>D3/G3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J3" t="e">
+        <f>D3/H3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K3" s="1">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>1100</v>
+      </c>
+      <c r="M3">
+        <v>390</v>
+      </c>
+      <c r="N3" s="1">
+        <v>10</v>
+      </c>
+      <c r="O3" s="2">
+        <v>10</v>
+      </c>
+      <c r="P3" s="2">
+        <v>10</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R3" s="1">
+        <v>125</v>
+      </c>
+      <c r="S3">
+        <v>1169</v>
+      </c>
+      <c r="T3">
+        <v>414</v>
+      </c>
+      <c r="U3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>32768</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="e">
+        <f>D4/G4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J4" t="e">
+        <f>D4/H4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K4" s="1">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>1100</v>
+      </c>
+      <c r="M4">
+        <v>390</v>
+      </c>
+      <c r="N4" s="1">
+        <v>26</v>
+      </c>
+      <c r="O4" s="2">
+        <v>70</v>
+      </c>
+      <c r="P4" s="2">
+        <v>25</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>61</v>
+      </c>
+      <c r="R4" s="1">
+        <v>125</v>
+      </c>
+      <c r="S4">
+        <v>1169</v>
+      </c>
+      <c r="T4">
+        <v>414</v>
+      </c>
+      <c r="U4" t="s">
+        <v>61</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="X4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>32768</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="e">
+        <f>D5/G5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J5" t="e">
+        <f>D5/H5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K5" s="1">
+        <v>100</v>
+      </c>
+      <c r="L5">
+        <v>1100</v>
+      </c>
+      <c r="M5">
+        <v>390</v>
+      </c>
+      <c r="N5" s="1">
+        <v>25</v>
+      </c>
+      <c r="O5" s="2">
+        <v>69</v>
+      </c>
+      <c r="P5" s="2">
+        <v>24</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" s="1">
+        <v>125</v>
+      </c>
+      <c r="S5">
+        <v>1169</v>
+      </c>
+      <c r="T5">
+        <v>414</v>
+      </c>
+      <c r="U5" t="s">
+        <v>61</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="X5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6">
+        <v>32768</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6" t="e">
+        <f>D6/G6</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J6" t="e">
+        <f>D6/H6</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K6" s="1">
+        <v>101</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1009</v>
+      </c>
+      <c r="M6" s="2">
+        <v>400</v>
+      </c>
+      <c r="N6" s="1">
+        <v>12</v>
+      </c>
+      <c r="O6" s="2">
+        <v>90</v>
+      </c>
+      <c r="P6" s="2">
+        <v>7</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R6" s="1">
+        <v>125</v>
+      </c>
+      <c r="S6">
+        <v>1169</v>
+      </c>
+      <c r="T6">
+        <v>414</v>
+      </c>
+      <c r="U6" t="s">
+        <v>61</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="X6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>32768</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" t="e">
+        <f>D7/G7</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J7" t="e">
+        <f>D7/H7</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K7" s="1">
+        <f>R7-50</f>
+        <v>75</v>
+      </c>
+      <c r="L7">
+        <f>S7-240</f>
+        <v>929</v>
+      </c>
+      <c r="M7">
+        <f>T7-110</f>
+        <v>304</v>
+      </c>
+      <c r="N7" s="1">
+        <f>(R7-K7)/2</f>
+        <v>25</v>
+      </c>
+      <c r="O7">
+        <f>(S7-L7)/2</f>
+        <v>120</v>
+      </c>
+      <c r="P7">
+        <f>(T7-M7)/2</f>
+        <v>55</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>61</v>
+      </c>
+      <c r="R7" s="1">
+        <v>125</v>
+      </c>
+      <c r="S7">
+        <v>1169</v>
+      </c>
+      <c r="T7">
+        <v>414</v>
+      </c>
+      <c r="U7" t="s">
+        <v>61</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="X7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>32768</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8" t="e">
+        <f>D8/G8</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J8" t="e">
+        <f>D8/H8</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K8" s="1">
+        <v>72</v>
+      </c>
+      <c r="L8">
+        <v>928</v>
+      </c>
+      <c r="M8">
+        <v>304</v>
+      </c>
+      <c r="N8" s="1">
+        <v>24</v>
+      </c>
+      <c r="O8">
+        <v>120</v>
+      </c>
+      <c r="P8">
+        <v>48</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>61</v>
+      </c>
+      <c r="R8" s="1">
+        <v>125</v>
+      </c>
+      <c r="S8">
+        <v>1169</v>
+      </c>
+      <c r="T8">
+        <v>414</v>
+      </c>
+      <c r="U8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="X8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9">
+        <v>32768</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9" t="e">
+        <f>D9/G9</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J9" t="e">
+        <f>D9/H9</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K9" s="1">
+        <v>64</v>
+      </c>
+      <c r="L9">
+        <v>928</v>
+      </c>
+      <c r="M9">
+        <v>304</v>
+      </c>
+      <c r="N9" s="1">
+        <v>24</v>
+      </c>
+      <c r="O9">
+        <v>120</v>
+      </c>
+      <c r="P9">
+        <v>40</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>61</v>
+      </c>
+      <c r="R9" s="1">
+        <v>125</v>
+      </c>
+      <c r="S9">
+        <v>1169</v>
+      </c>
+      <c r="T9">
+        <v>414</v>
+      </c>
+      <c r="U9" t="s">
+        <v>61</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="X9" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y9" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10">
+        <v>10135</v>
+      </c>
+      <c r="E10">
+        <v>32768</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="K10" s="1">
+        <v>64</v>
+      </c>
+      <c r="L10">
+        <v>400</v>
+      </c>
+      <c r="M10">
+        <v>160</v>
+      </c>
+      <c r="N10" s="1">
+        <v>24</v>
+      </c>
+      <c r="O10">
+        <v>376</v>
+      </c>
+      <c r="P10">
+        <v>120</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>61</v>
+      </c>
+      <c r="R10" s="1">
+        <v>125</v>
+      </c>
+      <c r="S10">
+        <v>1169</v>
+      </c>
+      <c r="T10">
+        <v>414</v>
+      </c>
+      <c r="U10" t="s">
+        <v>61</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W10" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>32768</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="K11" s="1">
+        <v>72</v>
+      </c>
+      <c r="L11">
+        <v>408</v>
+      </c>
+      <c r="M11">
+        <v>168</v>
+      </c>
+      <c r="N11" s="1">
+        <v>24</v>
+      </c>
+      <c r="O11">
+        <v>376</v>
+      </c>
+      <c r="P11">
+        <v>120</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>61</v>
+      </c>
+      <c r="R11" s="1">
+        <v>125</v>
+      </c>
+      <c r="S11">
+        <v>1169</v>
+      </c>
+      <c r="T11">
+        <v>414</v>
+      </c>
+      <c r="U11" t="s">
+        <v>61</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="X11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>32768</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="K12" s="1">
+        <v>72</v>
+      </c>
+      <c r="L12">
+        <v>408</v>
+      </c>
+      <c r="M12">
+        <v>168</v>
+      </c>
+      <c r="N12" s="1">
+        <v>16</v>
+      </c>
+      <c r="O12">
+        <v>368</v>
+      </c>
+      <c r="P12">
+        <v>112</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>61</v>
+      </c>
+      <c r="R12" s="1">
+        <v>125</v>
+      </c>
+      <c r="S12">
+        <v>1169</v>
+      </c>
+      <c r="T12">
+        <v>414</v>
+      </c>
+      <c r="U12" t="s">
+        <v>61</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="X12" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13">
+        <v>13843</v>
+      </c>
+      <c r="E13">
+        <v>32768</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="K13" s="1">
+        <v>80</v>
+      </c>
+      <c r="L13">
+        <v>416</v>
+      </c>
+      <c r="M13">
+        <v>176</v>
+      </c>
+      <c r="N13" s="1">
+        <v>8</v>
+      </c>
+      <c r="O13">
+        <v>376</v>
+      </c>
+      <c r="P13">
+        <v>104</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>61</v>
+      </c>
+      <c r="R13" s="1">
+        <v>125</v>
+      </c>
+      <c r="S13">
+        <v>1169</v>
+      </c>
+      <c r="T13">
+        <v>414</v>
+      </c>
+      <c r="U13" t="s">
+        <v>61</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W13" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14">
+        <v>13843</v>
+      </c>
+      <c r="E14">
+        <v>32768</v>
+      </c>
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="K14" s="1">
+        <v>80</v>
+      </c>
+      <c r="L14">
+        <v>416</v>
+      </c>
+      <c r="M14">
+        <v>176</v>
+      </c>
+      <c r="N14" s="1">
+        <v>16</v>
+      </c>
+      <c r="O14">
+        <v>368</v>
+      </c>
+      <c r="P14">
+        <v>112</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>61</v>
+      </c>
+      <c r="R14" s="1">
+        <v>125</v>
+      </c>
+      <c r="S14">
+        <v>1169</v>
+      </c>
+      <c r="T14">
+        <v>414</v>
+      </c>
+      <c r="U14" t="s">
+        <v>61</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W14" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="R15" s="1">
+        <v>125</v>
+      </c>
+      <c r="S15">
+        <v>1169</v>
+      </c>
+      <c r="T15">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="R16" s="1">
+        <v>125</v>
+      </c>
+      <c r="S16">
+        <v>1169</v>
+      </c>
+      <c r="T16">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="R17" s="1">
+        <v>125</v>
+      </c>
+      <c r="S17">
+        <v>1169</v>
+      </c>
+      <c r="T17">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R18" s="1">
+        <v>125</v>
+      </c>
+      <c r="S18">
+        <v>1169</v>
+      </c>
+      <c r="T18">
+        <v>414</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
complete today's VRAM study. copy valid sessions into separate file. cluster outputs copied to customer drive.
</commit_message>
<xml_diff>
--- a/VRAM patch stride table.xlsx
+++ b/VRAM patch stride table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7A13D2-90D4-4875-A3A5-7AE9AD08A3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5BD664-A4F7-4F3E-84CA-5E7879CD4EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="88">
   <si>
     <t>patch z</t>
   </si>
@@ -253,6 +253,54 @@
   </si>
   <si>
     <t>better performance metrics</t>
+  </si>
+  <si>
+    <t>230901-15</t>
+  </si>
+  <si>
+    <t>230901-16</t>
+  </si>
+  <si>
+    <t>230901-17</t>
+  </si>
+  <si>
+    <t>230901-18</t>
+  </si>
+  <si>
+    <t>VRAM ~ patch_shape study, common zyx</t>
+  </si>
+  <si>
+    <t>VRAM ~ patch_shape study, x change</t>
+  </si>
+  <si>
+    <t>VRAM ~ patch_shape study, y change</t>
+  </si>
+  <si>
+    <t>VRAM ~ patch_shape study, z change</t>
+  </si>
+  <si>
+    <t>2 patches per image, wanted 1</t>
+  </si>
+  <si>
+    <t>230901-19</t>
+  </si>
+  <si>
+    <t>TBD output transfer</t>
+  </si>
+  <si>
+    <t>patch = arbitrary even int_2^3</t>
+  </si>
+  <si>
+    <t>expectations/predictions</t>
+  </si>
+  <si>
+    <t>outcomes/evaluations</t>
+  </si>
+  <si>
+    <t>I expect the VRAM usage to be directly dependent on the difference in patch size.</t>
+  </si>
+  <si>
+    <t>I expect the same overall size (in pixels) to require the same amount of VRAM, if 3dunet truly has a 3D architecture (based on the best of my AI knowledge) - regardless of which dimension has what shape.</t>
   </si>
 </sst>
 </file>
@@ -290,7 +338,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -316,20 +364,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,1083 +733,1544 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:AD18"/>
+  <dimension ref="A1:AF24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875"/>
-    <col min="9" max="9" width="12.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="12.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="5.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.140625" customWidth="1"/>
-    <col min="13" max="13" width="5" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" customWidth="1"/>
-    <col min="16" max="17" width="5" customWidth="1"/>
-    <col min="18" max="18" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6" customWidth="1"/>
-    <col min="22" max="22" width="44" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="76.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="142" customWidth="1"/>
-    <col min="25" max="25" width="142" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="8.85546875"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="5.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="6.140625" customWidth="1"/>
+    <col min="15" max="16" width="5" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="6.5703125" customWidth="1"/>
+    <col min="19" max="19" width="5" customWidth="1"/>
+    <col min="20" max="20" width="6" customWidth="1"/>
+    <col min="21" max="21" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="34.28515625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="76.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="142" customWidth="1"/>
+    <col min="27" max="27" width="142" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="U1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Z1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>71</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>44</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>32768</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>43</v>
       </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2" t="e">
-        <f>D2/G2</f>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2" t="e">
+        <f t="shared" ref="K2:K9" si="0">F2/I2</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J2" t="e">
-        <f>D2/H2</f>
+      <c r="L2" t="e">
+        <f t="shared" ref="L2:L9" si="1">F2/J2</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K2" s="1">
+      <c r="M2" s="1">
         <v>105</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>1149</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>394</v>
       </c>
-      <c r="N2" s="1">
+      <c r="P2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="1">
         <v>10</v>
       </c>
-      <c r="O2">
+      <c r="R2">
         <v>10</v>
       </c>
-      <c r="P2">
+      <c r="S2">
         <v>10</v>
       </c>
-      <c r="Q2" t="s">
-        <v>61</v>
-      </c>
-      <c r="R2" s="1">
+      <c r="T2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" s="1">
         <v>125</v>
       </c>
-      <c r="S2">
+      <c r="V2">
         <v>1169</v>
       </c>
-      <c r="T2">
+      <c r="W2">
         <v>414</v>
       </c>
-      <c r="U2" t="s">
-        <v>61</v>
-      </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="Y2" t="s">
         <v>23</v>
       </c>
-      <c r="AB2">
-        <f>K2*L2*M2</f>
+      <c r="AD2">
+        <f>M2*N2*O2</f>
         <v>47534130</v>
       </c>
-      <c r="AC2">
+      <c r="AE2">
         <v>3</v>
       </c>
-      <c r="AD2">
-        <f>AB2*AC2</f>
+      <c r="AF2">
+        <f>AD2*AE2</f>
         <v>142602390</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>44</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>32768</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>43</v>
       </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
         <v>10</v>
       </c>
-      <c r="I3" t="e">
-        <f>D3/G3</f>
+      <c r="K3" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J3" t="e">
-        <f>D3/H3</f>
+      <c r="L3" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K3" s="1">
+      <c r="M3" s="1">
         <v>100</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>1100</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>390</v>
       </c>
-      <c r="N3" s="1">
+      <c r="P3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q3" s="1">
         <v>10</v>
       </c>
-      <c r="O3" s="2">
+      <c r="R3">
         <v>10</v>
       </c>
-      <c r="P3" s="2">
+      <c r="S3">
         <v>10</v>
       </c>
-      <c r="Q3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R3" s="1">
+      <c r="T3" t="s">
+        <v>61</v>
+      </c>
+      <c r="U3" s="1">
         <v>125</v>
       </c>
-      <c r="S3">
+      <c r="V3">
         <v>1169</v>
       </c>
-      <c r="T3">
+      <c r="W3">
         <v>414</v>
       </c>
-      <c r="U3" t="s">
-        <v>61</v>
-      </c>
-      <c r="V3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="Y3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>32768</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>43</v>
       </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
         <v>15</v>
       </c>
-      <c r="I4" t="e">
-        <f>D4/G4</f>
+      <c r="K4" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J4" t="e">
-        <f>D4/H4</f>
+      <c r="L4" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K4" s="1">
+      <c r="M4" s="1">
         <v>100</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>1100</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>390</v>
       </c>
-      <c r="N4" s="1">
+      <c r="P4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q4" s="1">
         <v>26</v>
       </c>
-      <c r="O4" s="2">
+      <c r="R4">
         <v>70</v>
       </c>
-      <c r="P4" s="2">
+      <c r="S4">
         <v>25</v>
       </c>
-      <c r="Q4" t="s">
-        <v>61</v>
-      </c>
-      <c r="R4" s="1">
+      <c r="T4" t="s">
+        <v>61</v>
+      </c>
+      <c r="U4" s="1">
         <v>125</v>
       </c>
-      <c r="S4">
+      <c r="V4">
         <v>1169</v>
       </c>
-      <c r="T4">
+      <c r="W4">
         <v>414</v>
       </c>
-      <c r="U4" t="s">
-        <v>61</v>
-      </c>
-      <c r="W4" s="5" t="s">
+      <c r="Y4" t="s">
         <v>17</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Z4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>32768</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>43</v>
       </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" t="e">
-        <f>D5/G5</f>
+      <c r="K5" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J5" t="e">
-        <f>D5/H5</f>
+      <c r="L5" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K5" s="1">
+      <c r="M5" s="1">
         <v>100</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>1100</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>390</v>
       </c>
-      <c r="N5" s="1">
+      <c r="P5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q5" s="1">
         <v>25</v>
       </c>
-      <c r="O5" s="2">
+      <c r="R5">
         <v>69</v>
       </c>
-      <c r="P5" s="2">
+      <c r="S5">
         <v>24</v>
       </c>
-      <c r="Q5" t="s">
-        <v>61</v>
-      </c>
-      <c r="R5" s="1">
+      <c r="T5" t="s">
+        <v>61</v>
+      </c>
+      <c r="U5" s="1">
         <v>125</v>
       </c>
-      <c r="S5">
+      <c r="V5">
         <v>1169</v>
       </c>
-      <c r="T5">
+      <c r="W5">
         <v>414</v>
       </c>
-      <c r="U5" t="s">
-        <v>61</v>
-      </c>
-      <c r="W5" s="5" t="s">
+      <c r="Y5" t="s">
         <v>16</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Z5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>44</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>32768</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>43</v>
       </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6" t="e">
-        <f>D6/G6</f>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J6" t="e">
-        <f>D6/H6</f>
+      <c r="L6" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K6" s="1">
+      <c r="M6" s="1">
         <v>101</v>
       </c>
-      <c r="L6" s="2">
+      <c r="N6">
         <v>1009</v>
       </c>
-      <c r="M6" s="2">
+      <c r="O6">
         <v>400</v>
       </c>
-      <c r="N6" s="1">
+      <c r="P6" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q6" s="1">
         <v>12</v>
       </c>
-      <c r="O6" s="2">
+      <c r="R6">
         <v>90</v>
       </c>
-      <c r="P6" s="2">
+      <c r="S6">
         <v>7</v>
       </c>
-      <c r="Q6" t="s">
-        <v>61</v>
-      </c>
-      <c r="R6" s="1">
+      <c r="T6" t="s">
+        <v>61</v>
+      </c>
+      <c r="U6" s="1">
         <v>125</v>
       </c>
-      <c r="S6">
+      <c r="V6">
         <v>1169</v>
       </c>
-      <c r="T6">
+      <c r="W6">
         <v>414</v>
       </c>
-      <c r="U6" t="s">
-        <v>61</v>
-      </c>
-      <c r="W6" s="5" t="s">
+      <c r="Y6" t="s">
         <v>23</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Z6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>15</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>32768</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>43</v>
       </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7" t="e">
-        <f>D7/G7</f>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J7" t="e">
-        <f>D7/H7</f>
+      <c r="L7" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K7" s="1">
-        <f>R7-50</f>
+      <c r="M7" s="1">
+        <f>U7-50</f>
         <v>75</v>
       </c>
-      <c r="L7">
-        <f>S7-240</f>
+      <c r="N7">
+        <f>V7-240</f>
         <v>929</v>
       </c>
-      <c r="M7">
-        <f>T7-110</f>
+      <c r="O7">
+        <f>W7-110</f>
         <v>304</v>
       </c>
-      <c r="N7" s="1">
-        <f>(R7-K7)/2</f>
+      <c r="P7" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q7" s="7">
+        <f>(U7-M7)/2</f>
         <v>25</v>
       </c>
-      <c r="O7">
-        <f>(S7-L7)/2</f>
+      <c r="R7" s="8">
+        <f>(V7-N7)/2</f>
         <v>120</v>
       </c>
-      <c r="P7">
-        <f>(T7-M7)/2</f>
+      <c r="S7" s="8">
+        <f>(W7-O7)/2</f>
         <v>55</v>
       </c>
-      <c r="Q7" t="s">
-        <v>61</v>
-      </c>
-      <c r="R7" s="1">
+      <c r="T7" t="s">
+        <v>61</v>
+      </c>
+      <c r="U7" s="1">
         <v>125</v>
       </c>
-      <c r="S7">
+      <c r="V7">
         <v>1169</v>
       </c>
-      <c r="T7">
+      <c r="W7">
         <v>414</v>
       </c>
-      <c r="U7" t="s">
-        <v>61</v>
-      </c>
-      <c r="V7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W7" s="5" t="s">
+      <c r="Y7" t="s">
         <v>23</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Z7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>15</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>32768</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>43</v>
       </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-      <c r="H8">
-        <v>5</v>
-      </c>
-      <c r="I8" t="e">
-        <f>D8/G8</f>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J8" t="e">
-        <f>D8/H8</f>
+      <c r="L8" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K8" s="1">
+      <c r="M8" s="1">
         <v>72</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>928</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>304</v>
       </c>
-      <c r="N8" s="1">
+      <c r="P8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q8" s="1">
         <v>24</v>
       </c>
-      <c r="O8">
+      <c r="R8">
         <v>120</v>
       </c>
-      <c r="P8">
+      <c r="S8">
         <v>48</v>
       </c>
-      <c r="Q8" t="s">
-        <v>61</v>
-      </c>
-      <c r="R8" s="1">
+      <c r="T8" t="s">
+        <v>61</v>
+      </c>
+      <c r="U8" s="1">
         <v>125</v>
       </c>
-      <c r="S8">
+      <c r="V8">
         <v>1169</v>
       </c>
-      <c r="T8">
+      <c r="W8">
         <v>414</v>
       </c>
-      <c r="U8" t="s">
-        <v>61</v>
-      </c>
-      <c r="V8" s="1" t="s">
+      <c r="X8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="W8" s="5" t="s">
+      <c r="Y8" t="s">
         <v>38</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Z8" t="s">
         <v>33</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AA8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>44</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>32768</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>43</v>
       </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
-      <c r="I9" t="e">
-        <f>D9/G9</f>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J9" t="e">
-        <f>D9/H9</f>
+      <c r="L9" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K9" s="1">
+      <c r="M9" s="1">
         <v>64</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>928</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>304</v>
       </c>
-      <c r="N9" s="1">
+      <c r="P9" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q9" s="1">
         <v>24</v>
       </c>
-      <c r="O9">
+      <c r="R9">
         <v>120</v>
       </c>
-      <c r="P9">
+      <c r="S9">
         <v>40</v>
       </c>
-      <c r="Q9" t="s">
-        <v>61</v>
-      </c>
-      <c r="R9" s="1">
+      <c r="T9" t="s">
+        <v>61</v>
+      </c>
+      <c r="U9" s="1">
         <v>125</v>
       </c>
-      <c r="S9">
+      <c r="V9">
         <v>1169</v>
       </c>
-      <c r="T9">
+      <c r="W9">
         <v>414</v>
       </c>
-      <c r="U9" t="s">
-        <v>61</v>
-      </c>
-      <c r="V9" s="1" t="s">
+      <c r="X9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="W9" s="5" t="s">
+      <c r="Y9" t="s">
         <v>39</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Z9" t="s">
         <v>40</v>
       </c>
-      <c r="Y9" s="6" t="s">
+      <c r="AA9" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>10135</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>32768</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>43</v>
       </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>5</v>
-      </c>
-      <c r="K10" s="1">
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="M10" s="1">
         <v>64</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>400</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>160</v>
       </c>
-      <c r="N10" s="1">
+      <c r="P10" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q10" s="1">
         <v>24</v>
       </c>
-      <c r="O10">
+      <c r="R10">
         <v>376</v>
       </c>
-      <c r="P10">
+      <c r="S10">
         <v>120</v>
       </c>
-      <c r="Q10" t="s">
-        <v>61</v>
-      </c>
-      <c r="R10" s="1">
+      <c r="T10" t="s">
+        <v>61</v>
+      </c>
+      <c r="U10" s="1">
         <v>125</v>
       </c>
-      <c r="S10">
+      <c r="V10">
         <v>1169</v>
       </c>
-      <c r="T10">
+      <c r="W10">
         <v>414</v>
       </c>
-      <c r="U10" t="s">
-        <v>61</v>
-      </c>
-      <c r="V10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="W10" s="5" t="s">
+      <c r="Y10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>52</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>60</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>15</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>32768</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>43</v>
       </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-      <c r="H11">
-        <v>5</v>
-      </c>
-      <c r="K11" s="1">
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="M11" s="1">
         <v>72</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>408</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>168</v>
       </c>
-      <c r="N11" s="1">
+      <c r="P11" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q11" s="1">
         <v>24</v>
       </c>
-      <c r="O11">
+      <c r="R11">
         <v>376</v>
       </c>
-      <c r="P11">
+      <c r="S11">
         <v>120</v>
       </c>
-      <c r="Q11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R11" s="1">
+      <c r="T11" t="s">
+        <v>61</v>
+      </c>
+      <c r="U11" s="1">
         <v>125</v>
       </c>
-      <c r="S11">
+      <c r="V11">
         <v>1169</v>
       </c>
-      <c r="T11">
+      <c r="W11">
         <v>414</v>
       </c>
-      <c r="U11" t="s">
-        <v>61</v>
-      </c>
-      <c r="V11" s="1" t="s">
+      <c r="X11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="W11" s="5" t="s">
+      <c r="Y11" t="s">
         <v>39</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Z11" t="s">
         <v>51</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="AA11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>53</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>60</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>15</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>32768</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>43</v>
       </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-      <c r="H12">
-        <v>5</v>
-      </c>
-      <c r="K12" s="1">
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="M12" s="1">
         <v>72</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>408</v>
       </c>
-      <c r="M12">
+      <c r="O12">
         <v>168</v>
       </c>
-      <c r="N12" s="1">
+      <c r="P12" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q12" s="1">
         <v>16</v>
       </c>
-      <c r="O12">
+      <c r="R12">
         <v>368</v>
       </c>
-      <c r="P12">
+      <c r="S12">
         <v>112</v>
       </c>
-      <c r="Q12" t="s">
-        <v>61</v>
-      </c>
-      <c r="R12" s="1">
+      <c r="T12" t="s">
+        <v>61</v>
+      </c>
+      <c r="U12" s="1">
         <v>125</v>
       </c>
-      <c r="S12">
+      <c r="V12">
         <v>1169</v>
       </c>
-      <c r="T12">
+      <c r="W12">
         <v>414</v>
       </c>
-      <c r="U12" t="s">
-        <v>61</v>
-      </c>
-      <c r="V12" s="1" t="s">
+      <c r="X12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="W12" s="5" t="s">
+      <c r="Y12" t="s">
         <v>59</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Z12" t="s">
         <v>51</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="AA12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13">
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13">
         <v>13843</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>32768</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>43</v>
       </c>
-      <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="H13">
-        <v>5</v>
-      </c>
-      <c r="K13" s="1">
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13">
+        <v>5</v>
+      </c>
+      <c r="M13" s="1">
         <v>80</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>416</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <v>176</v>
       </c>
-      <c r="N13" s="1">
+      <c r="P13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q13" s="1">
         <v>8</v>
       </c>
-      <c r="O13">
+      <c r="R13">
         <v>376</v>
       </c>
-      <c r="P13">
+      <c r="S13">
         <v>104</v>
       </c>
-      <c r="Q13" t="s">
-        <v>61</v>
-      </c>
-      <c r="R13" s="1">
+      <c r="T13" t="s">
+        <v>61</v>
+      </c>
+      <c r="U13" s="1">
         <v>125</v>
       </c>
-      <c r="S13">
+      <c r="V13">
         <v>1169</v>
       </c>
-      <c r="T13">
+      <c r="W13">
         <v>414</v>
       </c>
-      <c r="U13" t="s">
-        <v>61</v>
-      </c>
-      <c r="V13" s="1" t="s">
+      <c r="X13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="W13" s="5" t="s">
+      <c r="Y13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>55</v>
       </c>
-      <c r="C14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14">
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14">
         <v>13843</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>32768</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
         <v>43</v>
       </c>
-      <c r="G14">
-        <v>5</v>
-      </c>
-      <c r="H14">
-        <v>5</v>
-      </c>
-      <c r="K14" s="1">
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="M14" s="1">
         <v>80</v>
       </c>
-      <c r="L14">
+      <c r="N14">
         <v>416</v>
       </c>
-      <c r="M14">
+      <c r="O14">
         <v>176</v>
       </c>
-      <c r="N14" s="1">
+      <c r="P14" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q14" s="1">
         <v>16</v>
       </c>
-      <c r="O14">
+      <c r="R14">
         <v>368</v>
       </c>
-      <c r="P14">
+      <c r="S14">
         <v>112</v>
       </c>
-      <c r="Q14" t="s">
-        <v>61</v>
-      </c>
-      <c r="R14" s="1">
+      <c r="T14" t="s">
+        <v>61</v>
+      </c>
+      <c r="U14" s="1">
         <v>125</v>
       </c>
-      <c r="S14">
+      <c r="V14">
         <v>1169</v>
       </c>
-      <c r="T14">
+      <c r="W14">
         <v>414</v>
       </c>
-      <c r="U14" t="s">
-        <v>61</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="W14" s="5" t="s">
+      <c r="X14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="R15" s="1">
+      <c r="D15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="5">
+        <v>32768</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="5">
+        <v>5</v>
+      </c>
+      <c r="J15" s="15">
+        <v>10</v>
+      </c>
+      <c r="M15" s="6">
+        <v>64</v>
+      </c>
+      <c r="N15" s="5">
+        <v>400</v>
+      </c>
+      <c r="O15" s="5">
+        <v>160</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q15" s="14">
+        <v>8</v>
+      </c>
+      <c r="R15" s="11">
+        <v>368</v>
+      </c>
+      <c r="S15" s="11">
+        <v>96</v>
+      </c>
+      <c r="T15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="U15" s="6">
         <v>125</v>
       </c>
-      <c r="S15">
+      <c r="V15" s="5">
         <v>1169</v>
       </c>
-      <c r="T15">
+      <c r="W15" s="5">
         <v>414</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="X15" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
-      <c r="R16" s="1">
+      <c r="D16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16">
+        <v>10135</v>
+      </c>
+      <c r="G16" s="5">
+        <v>32768</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="13">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>5</v>
+      </c>
+      <c r="M16" s="1">
+        <v>64</v>
+      </c>
+      <c r="N16">
+        <v>400</v>
+      </c>
+      <c r="O16">
+        <v>160</v>
+      </c>
+      <c r="P16" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>24</v>
+      </c>
+      <c r="R16" s="10">
+        <v>384</v>
+      </c>
+      <c r="S16" s="10">
+        <v>120</v>
+      </c>
+      <c r="T16" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="U16" s="1">
         <v>125</v>
       </c>
-      <c r="S16">
+      <c r="V16" s="4">
         <v>1169</v>
       </c>
-      <c r="T16">
+      <c r="W16" s="4">
         <v>414</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X16" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
-      <c r="R17" s="1">
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17">
+        <v>10999</v>
+      </c>
+      <c r="G17">
+        <v>32768</v>
+      </c>
+      <c r="H17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <v>5</v>
+      </c>
+      <c r="M17" s="1">
+        <v>64</v>
+      </c>
+      <c r="N17">
+        <v>400</v>
+      </c>
+      <c r="O17">
+        <v>176</v>
+      </c>
+      <c r="P17" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>24</v>
+      </c>
+      <c r="R17" s="10">
+        <v>384</v>
+      </c>
+      <c r="S17" s="10">
+        <v>112</v>
+      </c>
+      <c r="T17" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="U17" s="1">
         <v>125</v>
       </c>
-      <c r="S17">
+      <c r="V17">
         <v>1169</v>
       </c>
-      <c r="T17">
+      <c r="W17">
         <v>414</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="R18" s="1">
+      <c r="X17" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18">
+        <v>11843</v>
+      </c>
+      <c r="G18">
+        <v>32768</v>
+      </c>
+      <c r="H18" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="M18" s="1">
+        <v>64</v>
+      </c>
+      <c r="N18">
+        <v>400</v>
+      </c>
+      <c r="O18">
+        <v>192</v>
+      </c>
+      <c r="P18" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>24</v>
+      </c>
+      <c r="R18" s="10">
+        <v>384</v>
+      </c>
+      <c r="S18" s="10">
+        <v>104</v>
+      </c>
+      <c r="T18" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="U18" s="1">
         <v>125</v>
       </c>
-      <c r="S18">
+      <c r="V18">
         <v>1169</v>
       </c>
-      <c r="T18">
+      <c r="W18">
         <v>414</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19">
+        <v>10473</v>
+      </c>
+      <c r="G19">
+        <v>32768</v>
+      </c>
+      <c r="H19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>5</v>
+      </c>
+      <c r="M19" s="1">
+        <v>64</v>
+      </c>
+      <c r="N19">
+        <v>416</v>
+      </c>
+      <c r="O19">
+        <v>160</v>
+      </c>
+      <c r="P19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>24</v>
+      </c>
+      <c r="R19" s="10">
+        <v>376</v>
+      </c>
+      <c r="S19" s="10">
+        <v>120</v>
+      </c>
+      <c r="T19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="U19" s="1">
+        <v>125</v>
+      </c>
+      <c r="V19">
+        <v>1169</v>
+      </c>
+      <c r="W19">
+        <v>414</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20">
+        <v>10825</v>
+      </c>
+      <c r="G20">
+        <v>32768</v>
+      </c>
+      <c r="H20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+      <c r="M20" s="1">
+        <v>64</v>
+      </c>
+      <c r="N20">
+        <v>432</v>
+      </c>
+      <c r="O20">
+        <v>160</v>
+      </c>
+      <c r="P20" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q20" s="9">
+        <v>24</v>
+      </c>
+      <c r="R20" s="10">
+        <v>368</v>
+      </c>
+      <c r="S20" s="10">
+        <v>120</v>
+      </c>
+      <c r="T20" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="U20" s="1">
+        <v>125</v>
+      </c>
+      <c r="V20">
+        <v>1169</v>
+      </c>
+      <c r="W20">
+        <v>414</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21">
+        <v>12317</v>
+      </c>
+      <c r="G21">
+        <v>32768</v>
+      </c>
+      <c r="H21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="M21" s="9">
+        <v>80</v>
+      </c>
+      <c r="N21" s="10">
+        <v>400</v>
+      </c>
+      <c r="O21" s="10">
+        <v>160</v>
+      </c>
+      <c r="P21" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q21" s="9">
+        <v>16</v>
+      </c>
+      <c r="R21" s="10">
+        <v>384</v>
+      </c>
+      <c r="S21" s="10">
+        <v>120</v>
+      </c>
+      <c r="T21" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="U21" s="1">
+        <v>125</v>
+      </c>
+      <c r="V21">
+        <v>1169</v>
+      </c>
+      <c r="W21">
+        <v>414</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22">
+        <v>14443</v>
+      </c>
+      <c r="G22">
+        <v>32768</v>
+      </c>
+      <c r="H22" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+      <c r="M22" s="9">
+        <v>96</v>
+      </c>
+      <c r="N22" s="10">
+        <v>400</v>
+      </c>
+      <c r="O22" s="10">
+        <v>160</v>
+      </c>
+      <c r="P22" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q22" s="9">
+        <v>8</v>
+      </c>
+      <c r="R22" s="10">
+        <v>384</v>
+      </c>
+      <c r="S22" s="10">
+        <v>120</v>
+      </c>
+      <c r="T22" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="U22" s="1">
+        <v>125</v>
+      </c>
+      <c r="V22">
+        <v>1169</v>
+      </c>
+      <c r="W22">
+        <v>414</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create VRAM analysis R script. finish data wrangling
</commit_message>
<xml_diff>
--- a/VRAM patch stride table.xlsx
+++ b/VRAM patch stride table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A98E99-82A8-4B2A-BEDD-91A00AA34CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219F25A9-56B7-49FA-9275-C89495AF8FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="115">
   <si>
     <t>patch z</t>
   </si>
@@ -261,9 +261,6 @@
     <t>230901-19</t>
   </si>
   <si>
-    <t>TBD output transfer</t>
-  </si>
-  <si>
     <t>patch = arbitrary even int_2^3</t>
   </si>
   <si>
@@ -376,6 +373,15 @@
   </si>
   <si>
     <t>raw pixel type</t>
+  </si>
+  <si>
+    <t>VRAM usage just below GPU capacity (gut feeling estimation)</t>
+  </si>
+  <si>
+    <t>better performance metrics due to raw channel being 16 bit now instead of 8 bit as previously (dataset02, multichannel babb03)</t>
+  </si>
+  <si>
+    <t>230901-12 to 230901-19</t>
   </si>
 </sst>
 </file>
@@ -511,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -525,14 +531,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,7 +854,7 @@
   <dimension ref="A1:AN24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -878,8 +882,8 @@
     <col min="30" max="30" width="5" customWidth="1"/>
     <col min="31" max="31" width="6" customWidth="1"/>
     <col min="32" max="32" width="34.28515625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="61.42578125" customWidth="1"/>
-    <col min="34" max="34" width="51.42578125" customWidth="1"/>
+    <col min="33" max="33" width="131.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="47" customWidth="1"/>
     <col min="36" max="36" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -896,46 +900,46 @@
         <v>62</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>61</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="N1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="N1" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="O1" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="P1" s="17" t="s">
-        <v>110</v>
+      <c r="P1" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>4</v>
@@ -971,18 +975,18 @@
         <v>57</v>
       </c>
       <c r="AB1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="AE1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="8" t="s">
         <v>24</v>
       </c>
       <c r="AG1" s="2" t="s">
@@ -1002,8 +1006,11 @@
       <c r="B2" t="s">
         <v>63</v>
       </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1012,7 +1019,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H2">
         <v>5</v>
@@ -1033,13 +1040,13 @@
         <v>16</v>
       </c>
       <c r="N2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O2">
         <v>8</v>
       </c>
       <c r="P2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q2">
         <v>5</v>
@@ -1091,6 +1098,12 @@
       </c>
       <c r="AG2" t="s">
         <v>16</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
@@ -1100,8 +1113,11 @@
       <c r="B3" t="s">
         <v>59</v>
       </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1110,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H3">
         <v>5</v>
@@ -1131,13 +1147,13 @@
         <v>16</v>
       </c>
       <c r="N3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O3">
         <v>8</v>
       </c>
       <c r="P3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q3">
         <v>10</v>
@@ -1189,6 +1205,12 @@
       </c>
       <c r="AG3" t="s">
         <v>16</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
@@ -1196,13 +1218,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1211,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -1232,13 +1254,13 @@
         <v>16</v>
       </c>
       <c r="N4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O4">
         <v>8</v>
       </c>
       <c r="P4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q4" t="s">
         <v>8</v>
@@ -1293,6 +1315,9 @@
       </c>
       <c r="AH4" t="s">
         <v>15</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -1300,13 +1325,13 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1315,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H5">
         <v>5</v>
@@ -1336,13 +1361,13 @@
         <v>16</v>
       </c>
       <c r="N5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O5">
         <v>8</v>
       </c>
       <c r="P5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q5" t="s">
         <v>8</v>
@@ -1397,6 +1422,9 @@
       </c>
       <c r="AH5" t="s">
         <v>15</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
@@ -1404,13 +1432,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1419,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -1440,13 +1468,13 @@
         <v>16</v>
       </c>
       <c r="N6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O6">
         <v>8</v>
       </c>
       <c r="P6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q6">
         <v>5</v>
@@ -1511,7 +1539,7 @@
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1520,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H7">
         <v>5</v>
@@ -1541,13 +1569,13 @@
         <v>16</v>
       </c>
       <c r="N7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O7">
         <v>8</v>
       </c>
       <c r="P7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q7">
         <v>5</v>
@@ -1608,6 +1636,9 @@
       </c>
       <c r="AH7" t="s">
         <v>26</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
@@ -1615,13 +1646,13 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
         <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1630,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H8">
         <v>5</v>
@@ -1651,13 +1682,13 @@
         <v>16</v>
       </c>
       <c r="N8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O8">
         <v>8</v>
       </c>
       <c r="P8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q8">
         <v>5</v>
@@ -1708,7 +1739,7 @@
         <v>30</v>
       </c>
       <c r="AG8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AH8" t="s">
         <v>26</v>
@@ -1717,18 +1748,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1737,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H9">
         <v>5</v>
@@ -1758,13 +1789,13 @@
         <v>16</v>
       </c>
       <c r="N9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O9">
         <v>8</v>
       </c>
       <c r="P9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q9">
         <v>5</v>
@@ -1829,7 +1860,7 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
         <v>53</v>
@@ -1844,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H10">
         <v>5</v>
@@ -1865,13 +1896,13 @@
         <v>16</v>
       </c>
       <c r="N10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O10">
         <v>8</v>
       </c>
       <c r="P10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q10">
         <v>5</v>
@@ -1923,6 +1954,12 @@
       </c>
       <c r="AG10" t="s">
         <v>31</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
@@ -1933,7 +1970,7 @@
         <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D11" t="s">
         <v>52</v>
@@ -1945,7 +1982,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H11">
         <v>5</v>
@@ -1966,13 +2003,13 @@
         <v>16</v>
       </c>
       <c r="N11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O11">
         <v>8</v>
       </c>
       <c r="P11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q11">
         <v>5</v>
@@ -2040,7 +2077,7 @@
         <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" t="s">
         <v>52</v>
@@ -2052,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H12">
         <v>5</v>
@@ -2073,13 +2110,13 @@
         <v>16</v>
       </c>
       <c r="N12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O12">
         <v>8</v>
       </c>
       <c r="P12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q12">
         <v>5</v>
@@ -2147,7 +2184,7 @@
         <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D13" t="s">
         <v>53</v>
@@ -2159,7 +2196,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H13">
         <v>5</v>
@@ -2180,13 +2217,13 @@
         <v>16</v>
       </c>
       <c r="N13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O13">
         <v>8</v>
       </c>
       <c r="P13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q13">
         <v>5</v>
@@ -2238,6 +2275,12 @@
       </c>
       <c r="AG13" t="s">
         <v>31</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -2248,7 +2291,7 @@
         <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D14" t="s">
         <v>53</v>
@@ -2260,7 +2303,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H14">
         <v>5</v>
@@ -2281,13 +2324,13 @@
         <v>16</v>
       </c>
       <c r="N14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O14">
         <v>8</v>
       </c>
       <c r="P14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q14">
         <v>5</v>
@@ -2295,10 +2338,10 @@
       <c r="R14">
         <v>13843</v>
       </c>
-      <c r="S14" s="12">
+      <c r="S14">
         <v>32768</v>
       </c>
-      <c r="T14" s="12" t="s">
+      <c r="T14" t="s">
         <v>35</v>
       </c>
       <c r="U14" s="1">
@@ -2335,10 +2378,16 @@
         <v>53</v>
       </c>
       <c r="AF14" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AG14" t="s">
         <v>51</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2348,20 +2397,20 @@
       <c r="B15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>101</v>
+      <c r="C15" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="4">
         <v>0</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="4">
         <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H15" s="4">
         <v>5</v>
@@ -2382,19 +2431,19 @@
         <v>16</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O15" s="4">
         <v>8</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q15" s="10">
         <v>10</v>
       </c>
-      <c r="R15" s="4" t="s">
-        <v>74</v>
+      <c r="R15" s="4">
+        <v>10135</v>
       </c>
       <c r="S15" s="4">
         <v>32768</v>
@@ -2436,10 +2485,16 @@
         <v>53</v>
       </c>
       <c r="AF15" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AG15" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="AH15" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI15" s="15" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -2449,20 +2504,20 @@
       <c r="B16" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="16">
+      <c r="C16" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H16">
         <v>5</v>
@@ -2483,13 +2538,13 @@
         <v>16</v>
       </c>
       <c r="N16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O16">
         <v>8</v>
       </c>
       <c r="P16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q16">
         <v>5</v>
@@ -2497,10 +2552,10 @@
       <c r="R16">
         <v>10135</v>
       </c>
-      <c r="S16" s="12">
+      <c r="S16">
         <v>32768</v>
       </c>
-      <c r="T16" s="12" t="s">
+      <c r="T16" t="s">
         <v>35</v>
       </c>
       <c r="U16" s="1">
@@ -2537,33 +2592,39 @@
         <v>53</v>
       </c>
       <c r="AF16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AG16" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="AH16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI16" s="14" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
       <c r="B17" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="16">
+      <c r="C17" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17">
         <v>5</v>
@@ -2584,13 +2645,13 @@
         <v>16</v>
       </c>
       <c r="N17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O17">
         <v>8</v>
       </c>
       <c r="P17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q17">
         <v>5</v>
@@ -2598,10 +2659,10 @@
       <c r="R17">
         <v>10999</v>
       </c>
-      <c r="S17" s="12">
+      <c r="S17">
         <v>32768</v>
       </c>
-      <c r="T17" s="12" t="s">
+      <c r="T17" t="s">
         <v>35</v>
       </c>
       <c r="U17" s="1">
@@ -2638,33 +2699,39 @@
         <v>53</v>
       </c>
       <c r="AF17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AG17" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="AH17" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI17" s="14" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
       <c r="B18" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="16">
+      <c r="C18" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H18">
         <v>5</v>
@@ -2685,13 +2752,13 @@
         <v>16</v>
       </c>
       <c r="N18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O18">
         <v>8</v>
       </c>
       <c r="P18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q18">
         <v>5</v>
@@ -2739,33 +2806,39 @@
         <v>53</v>
       </c>
       <c r="AF18" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AG18" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="AH18" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI18" s="14" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
       <c r="B19" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="16">
+      <c r="C19" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H19">
         <v>5</v>
@@ -2786,13 +2859,13 @@
         <v>16</v>
       </c>
       <c r="N19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O19">
         <v>8</v>
       </c>
       <c r="P19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q19">
         <v>5</v>
@@ -2840,33 +2913,39 @@
         <v>53</v>
       </c>
       <c r="AF19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AG19" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="AH19" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI19" s="14" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>66</v>
       </c>
       <c r="B20" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="16">
+      <c r="C20" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H20">
         <v>5</v>
@@ -2887,13 +2966,13 @@
         <v>16</v>
       </c>
       <c r="N20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O20">
         <v>8</v>
       </c>
       <c r="P20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q20">
         <v>5</v>
@@ -2941,33 +3020,39 @@
         <v>53</v>
       </c>
       <c r="AF20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AG20" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="AH20" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI20" s="14" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>67</v>
       </c>
       <c r="B21" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="16">
+      <c r="C21" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H21">
         <v>5</v>
@@ -2988,13 +3073,13 @@
         <v>16</v>
       </c>
       <c r="N21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O21">
         <v>8</v>
       </c>
       <c r="P21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q21">
         <v>5</v>
@@ -3042,33 +3127,39 @@
         <v>53</v>
       </c>
       <c r="AF21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AG21" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="AH21" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI21" s="14" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>73</v>
       </c>
       <c r="B22" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="16">
+      <c r="C22" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H22">
         <v>5</v>
@@ -3089,13 +3180,13 @@
         <v>16</v>
       </c>
       <c r="N22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O22">
         <v>8</v>
       </c>
       <c r="P22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q22">
         <v>5</v>
@@ -3143,20 +3234,230 @@
         <v>53</v>
       </c>
       <c r="AF22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AG22" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="AH22" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI22" s="14" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C23" s="14" t="s">
-        <v>78</v>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="R23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="S23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="T23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="U23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="V23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="W23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="X23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI23" s="14" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C24" s="15" t="s">
-        <v>77</v>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="R24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="S24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="T24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="U24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="V24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="W24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="X24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI24" s="14" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update VRAM script & excel table with VRAM usage predictions
</commit_message>
<xml_diff>
--- a/VRAM patch stride table.xlsx
+++ b/VRAM patch stride table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219F25A9-56B7-49FA-9275-C89495AF8FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE641904-7DF7-4885-8F40-BD67E4228A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="126">
   <si>
     <t>patch z</t>
   </si>
@@ -270,9 +270,6 @@
     <t>I expect the same overall size (in pixels) to require the same amount of VRAM, if 3dunet truly has a 3D architecture (based on the best of my AI knowledge) - regardless of which dimension has what shape.</t>
   </si>
   <si>
-    <t>I expect the VRAM usage to be directly, but not linearly, dependent on the difference in patch size.</t>
-  </si>
-  <si>
     <t>dataset</t>
   </si>
   <si>
@@ -382,6 +379,42 @@
   </si>
   <si>
     <t>230901-12 to 230901-19</t>
+  </si>
+  <si>
+    <t>230905-0</t>
+  </si>
+  <si>
+    <t>test VRAM prediction</t>
+  </si>
+  <si>
+    <t>I expect the VRAM usage to be directly, but not linearly, dependent on the difference in patch size (volume).</t>
+  </si>
+  <si>
+    <t>VRAM usage is linearly dependent on patch size (volume).</t>
+  </si>
+  <si>
+    <t>This is the case. The linear relationship between VRAM usage and only the patch volume (z * y * x pixels) is very strong, i.e., p &lt; 2e-16</t>
+  </si>
+  <si>
+    <t>predicted VRAM usage (MiB)</t>
+  </si>
+  <si>
+    <t>230905-1</t>
+  </si>
+  <si>
+    <t>test VRAM prediction, better performance metrics</t>
+  </si>
+  <si>
+    <t>NVIDIA A100-SXM4-80GB</t>
+  </si>
+  <si>
+    <t>expect VRAM ~ patch volume, expect VRAM to suffice</t>
+  </si>
+  <si>
+    <t>expect VRAM ~ patch volume, expect out of VRAM error</t>
+  </si>
+  <si>
+    <t>stride = foor (resolution - patch) / 2</t>
   </si>
 </sst>
 </file>
@@ -517,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -534,9 +567,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,48 +885,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:AN24"/>
+  <dimension ref="A1:AO36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.85546875" customWidth="1"/>
     <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="5.140625" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" customWidth="1"/>
-    <col min="15" max="16" width="5.140625" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" customWidth="1"/>
-    <col min="19" max="19" width="7.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="22.140625" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.28515625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="6.140625" customWidth="1"/>
-    <col min="26" max="27" width="5" customWidth="1"/>
-    <col min="28" max="28" width="6.140625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="6.5703125" customWidth="1"/>
-    <col min="30" max="30" width="5" customWidth="1"/>
-    <col min="31" max="31" width="6" customWidth="1"/>
-    <col min="32" max="32" width="34.28515625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="131.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="47" customWidth="1"/>
-    <col min="36" max="36" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="12.140625" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="9.5703125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="6.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="13" width="5.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="8.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="16" width="5.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="9.140625" collapsed="1"/>
+    <col min="18" max="19" width="9.140625" customWidth="1"/>
+    <col min="20" max="20" width="7.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="23.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.28515625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" customWidth="1"/>
+    <col min="27" max="28" width="5" customWidth="1"/>
+    <col min="29" max="29" width="6.140625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="6.5703125" customWidth="1"/>
+    <col min="31" max="31" width="5" customWidth="1"/>
+    <col min="32" max="32" width="6" customWidth="1"/>
+    <col min="33" max="33" width="34.28515625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="131.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="47" customWidth="1"/>
+    <col min="37" max="37" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="41" max="41" width="12.140625" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
@@ -906,40 +941,40 @@
         <v>61</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="P1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>4</v>
@@ -948,58 +983,61 @@
         <v>42</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AD1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AG1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -1007,10 +1045,10 @@
         <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1019,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H2">
         <v>5</v>
@@ -1040,13 +1078,13 @@
         <v>16</v>
       </c>
       <c r="N2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O2">
         <v>8</v>
       </c>
       <c r="P2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q2">
         <v>5</v>
@@ -1054,59 +1092,62 @@
       <c r="R2" t="s">
         <v>36</v>
       </c>
-      <c r="S2">
+      <c r="S2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2">
         <v>32768</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="1">
+      <c r="V2" s="1">
         <v>125</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>1169</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>414</v>
       </c>
-      <c r="X2" s="1">
+      <c r="Y2" s="1">
         <v>105</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>1149</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>394</v>
       </c>
-      <c r="AA2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>10</v>
-      </c>
-      <c r="AC2">
+      <c r="AB2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC2" s="1">
         <v>10</v>
       </c>
       <c r="AD2">
         <v>10</v>
       </c>
-      <c r="AE2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AE2">
+        <v>10</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>16</v>
       </c>
-      <c r="AH2" t="s">
-        <v>8</v>
-      </c>
       <c r="AI2" t="s">
         <v>8</v>
       </c>
+      <c r="AJ2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1114,10 +1155,10 @@
         <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1126,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H3">
         <v>5</v>
@@ -1147,13 +1188,13 @@
         <v>16</v>
       </c>
       <c r="N3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O3">
         <v>8</v>
       </c>
       <c r="P3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q3">
         <v>10</v>
@@ -1161,70 +1202,73 @@
       <c r="R3" t="s">
         <v>36</v>
       </c>
-      <c r="S3">
+      <c r="S3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3">
         <v>32768</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>35</v>
       </c>
-      <c r="U3" s="1">
+      <c r="V3" s="1">
         <v>125</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>1169</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>414</v>
       </c>
-      <c r="X3" s="1">
+      <c r="Y3" s="1">
         <v>100</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>1100</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>390</v>
       </c>
-      <c r="AA3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AC3">
+      <c r="AB3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC3" s="1">
         <v>10</v>
       </c>
       <c r="AD3">
         <v>10</v>
       </c>
-      <c r="AE3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AE3">
+        <v>10</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>16</v>
       </c>
-      <c r="AH3" t="s">
-        <v>8</v>
-      </c>
       <c r="AI3" t="s">
         <v>8</v>
       </c>
+      <c r="AJ3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1233,7 +1277,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -1254,13 +1298,13 @@
         <v>16</v>
       </c>
       <c r="N4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O4">
         <v>8</v>
       </c>
       <c r="P4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q4" t="s">
         <v>8</v>
@@ -1268,70 +1312,73 @@
       <c r="R4" t="s">
         <v>8</v>
       </c>
-      <c r="S4">
+      <c r="S4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4">
         <v>32768</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>35</v>
       </c>
-      <c r="U4" s="1">
+      <c r="V4" s="1">
         <v>125</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>1169</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>414</v>
       </c>
-      <c r="X4" s="1">
+      <c r="Y4" s="1">
         <v>100</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>1100</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>390</v>
       </c>
-      <c r="AA4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB4" s="1">
+      <c r="AB4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC4" s="1">
         <v>26</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>70</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>25</v>
       </c>
-      <c r="AE4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AF4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>10</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>15</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1340,7 +1387,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5">
         <v>5</v>
@@ -1361,13 +1408,13 @@
         <v>16</v>
       </c>
       <c r="N5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O5">
         <v>8</v>
       </c>
       <c r="P5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q5" t="s">
         <v>8</v>
@@ -1375,70 +1422,73 @@
       <c r="R5" t="s">
         <v>8</v>
       </c>
-      <c r="S5">
+      <c r="S5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5">
         <v>32768</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>35</v>
       </c>
-      <c r="U5" s="1">
+      <c r="V5" s="1">
         <v>125</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>1169</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>414</v>
       </c>
-      <c r="X5" s="1">
+      <c r="Y5" s="1">
         <v>100</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>1100</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>390</v>
       </c>
-      <c r="AA5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB5" s="1">
+      <c r="AB5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC5" s="1">
         <v>25</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>69</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>24</v>
       </c>
-      <c r="AE5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AF5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>9</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>15</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1447,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -1468,13 +1518,13 @@
         <v>16</v>
       </c>
       <c r="N6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O6">
         <v>8</v>
       </c>
       <c r="P6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q6">
         <v>5</v>
@@ -1482,56 +1532,59 @@
       <c r="R6" t="s">
         <v>36</v>
       </c>
-      <c r="S6">
+      <c r="S6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T6">
         <v>32768</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>35</v>
       </c>
-      <c r="U6" s="1">
+      <c r="V6" s="1">
         <v>125</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>1169</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>414</v>
       </c>
-      <c r="X6" s="1">
+      <c r="Y6" s="1">
         <v>101</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>1009</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <v>400</v>
       </c>
-      <c r="AA6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB6" s="1">
+      <c r="AB6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC6" s="1">
         <v>12</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>90</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>7</v>
       </c>
-      <c r="AE6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF6" s="1" t="s">
+      <c r="AF6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>16</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1539,7 +1592,7 @@
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1548,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H7">
         <v>5</v>
@@ -1569,13 +1622,13 @@
         <v>16</v>
       </c>
       <c r="N7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O7">
         <v>8</v>
       </c>
       <c r="P7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q7">
         <v>5</v>
@@ -1583,76 +1636,79 @@
       <c r="R7" t="s">
         <v>8</v>
       </c>
-      <c r="S7">
+      <c r="S7" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7">
         <v>32768</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>35</v>
       </c>
-      <c r="U7" s="1">
+      <c r="V7" s="1">
         <v>125</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>1169</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>414</v>
       </c>
-      <c r="X7" s="1">
-        <f>U7-50</f>
+      <c r="Y7" s="1">
+        <f>V7-50</f>
         <v>75</v>
       </c>
-      <c r="Y7">
-        <f>V7-240</f>
+      <c r="Z7">
+        <f>W7-240</f>
         <v>929</v>
       </c>
-      <c r="Z7">
-        <f>W7-110</f>
+      <c r="AA7">
+        <f>X7-110</f>
         <v>304</v>
       </c>
-      <c r="AA7" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB7" s="6">
-        <f>(U7-X7)/2</f>
+      <c r="AB7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC7" s="6">
+        <f>(V7-Y7)/2</f>
         <v>25</v>
-      </c>
-      <c r="AC7" s="7">
-        <f>(V7-Y7)/2</f>
-        <v>120</v>
       </c>
       <c r="AD7" s="7">
         <f>(W7-Z7)/2</f>
+        <v>120</v>
+      </c>
+      <c r="AE7" s="7">
+        <f>(X7-AA7)/2</f>
         <v>55</v>
       </c>
-      <c r="AE7" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AF7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>16</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AI7" t="s">
         <v>26</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
         <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1661,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H8">
         <v>5</v>
@@ -1682,13 +1738,13 @@
         <v>16</v>
       </c>
       <c r="N8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O8">
         <v>8</v>
       </c>
       <c r="P8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q8">
         <v>5</v>
@@ -1696,70 +1752,73 @@
       <c r="R8" t="s">
         <v>8</v>
       </c>
-      <c r="S8">
+      <c r="S8" t="s">
+        <v>8</v>
+      </c>
+      <c r="T8">
         <v>32768</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>35</v>
       </c>
-      <c r="U8" s="1">
+      <c r="V8" s="1">
         <v>125</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>1169</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>414</v>
       </c>
-      <c r="X8" s="1">
+      <c r="Y8" s="1">
         <v>72</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>928</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <v>304</v>
       </c>
-      <c r="AA8" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB8" s="1">
+      <c r="AB8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC8" s="1">
         <v>24</v>
       </c>
-      <c r="AC8">
+      <c r="AD8">
         <v>120</v>
       </c>
-      <c r="AD8">
+      <c r="AE8">
         <v>48</v>
       </c>
-      <c r="AE8" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF8" s="1" t="s">
+      <c r="AF8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG8" t="s">
-        <v>81</v>
-      </c>
       <c r="AH8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI8" t="s">
         <v>26</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="AJ8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1768,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H9">
         <v>5</v>
@@ -1789,13 +1848,13 @@
         <v>16</v>
       </c>
       <c r="N9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O9">
         <v>8</v>
       </c>
       <c r="P9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q9">
         <v>5</v>
@@ -1803,64 +1862,67 @@
       <c r="R9" t="s">
         <v>36</v>
       </c>
-      <c r="S9">
+      <c r="S9" t="s">
+        <v>8</v>
+      </c>
+      <c r="T9">
         <v>32768</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>35</v>
       </c>
-      <c r="U9" s="1">
+      <c r="V9" s="1">
         <v>125</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>1169</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>414</v>
       </c>
-      <c r="X9" s="1">
+      <c r="Y9" s="1">
         <v>64</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>928</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <v>304</v>
       </c>
-      <c r="AA9" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB9" s="1">
+      <c r="AB9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC9" s="1">
         <v>24</v>
       </c>
-      <c r="AC9">
+      <c r="AD9">
         <v>120</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>40</v>
       </c>
-      <c r="AE9" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF9" s="1" t="s">
+      <c r="AF9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AH9" t="s">
         <v>31</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AI9" t="s">
         <v>32</v>
       </c>
-      <c r="AI9" s="3" t="s">
+      <c r="AJ9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
         <v>53</v>
@@ -1875,7 +1937,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H10">
         <v>5</v>
@@ -1896,13 +1958,13 @@
         <v>16</v>
       </c>
       <c r="N10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O10">
         <v>8</v>
       </c>
       <c r="P10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q10">
         <v>5</v>
@@ -1910,59 +1972,62 @@
       <c r="R10">
         <v>10135</v>
       </c>
-      <c r="S10">
+      <c r="S10" t="s">
+        <v>8</v>
+      </c>
+      <c r="T10">
         <v>32768</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>35</v>
       </c>
-      <c r="U10" s="1">
+      <c r="V10" s="1">
         <v>125</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>1169</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>414</v>
       </c>
-      <c r="X10" s="1">
+      <c r="Y10" s="1">
         <v>64</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>400</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <v>160</v>
       </c>
-      <c r="AA10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB10" s="1">
+      <c r="AB10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC10" s="1">
         <v>24</v>
       </c>
-      <c r="AC10">
+      <c r="AD10">
         <v>376</v>
       </c>
-      <c r="AD10">
+      <c r="AE10">
         <v>120</v>
       </c>
-      <c r="AE10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF10" s="1" t="s">
+      <c r="AF10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AG10" t="s">
+      <c r="AH10" t="s">
         <v>31</v>
       </c>
-      <c r="AH10" t="s">
-        <v>8</v>
-      </c>
       <c r="AI10" t="s">
         <v>8</v>
       </c>
+      <c r="AJ10" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1970,7 +2035,7 @@
         <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" t="s">
         <v>52</v>
@@ -1982,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H11">
         <v>5</v>
@@ -2003,13 +2068,13 @@
         <v>16</v>
       </c>
       <c r="N11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O11">
         <v>8</v>
       </c>
       <c r="P11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q11">
         <v>5</v>
@@ -2017,59 +2082,62 @@
       <c r="R11" t="s">
         <v>8</v>
       </c>
-      <c r="S11">
+      <c r="S11" t="s">
+        <v>8</v>
+      </c>
+      <c r="T11">
         <v>32768</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>35</v>
       </c>
-      <c r="U11" s="1">
+      <c r="V11" s="1">
         <v>125</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>1169</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>414</v>
       </c>
-      <c r="X11" s="1">
+      <c r="Y11" s="1">
         <v>72</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>408</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>168</v>
       </c>
-      <c r="AA11" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB11" s="1">
+      <c r="AB11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC11" s="1">
         <v>24</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>376</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <v>120</v>
       </c>
-      <c r="AE11" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF11" s="1" t="s">
+      <c r="AF11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AH11" t="s">
         <v>31</v>
       </c>
-      <c r="AH11" t="s">
+      <c r="AI11" t="s">
         <v>43</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AJ11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -2077,7 +2145,7 @@
         <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" t="s">
         <v>52</v>
@@ -2089,7 +2157,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H12">
         <v>5</v>
@@ -2110,13 +2178,13 @@
         <v>16</v>
       </c>
       <c r="N12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O12">
         <v>8</v>
       </c>
       <c r="P12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q12">
         <v>5</v>
@@ -2124,59 +2192,62 @@
       <c r="R12" t="s">
         <v>8</v>
       </c>
-      <c r="S12">
+      <c r="S12" t="s">
+        <v>8</v>
+      </c>
+      <c r="T12">
         <v>32768</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>35</v>
       </c>
-      <c r="U12" s="1">
+      <c r="V12" s="1">
         <v>125</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>1169</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>414</v>
       </c>
-      <c r="X12" s="1">
+      <c r="Y12" s="1">
         <v>72</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>408</v>
       </c>
-      <c r="Z12">
+      <c r="AA12">
         <v>168</v>
       </c>
-      <c r="AA12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB12" s="1">
+      <c r="AB12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC12" s="1">
         <v>16</v>
       </c>
-      <c r="AC12">
+      <c r="AD12">
         <v>368</v>
       </c>
-      <c r="AD12">
+      <c r="AE12">
         <v>112</v>
       </c>
-      <c r="AE12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF12" s="1" t="s">
+      <c r="AF12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AG12" t="s">
+      <c r="AH12" t="s">
         <v>51</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AI12" t="s">
         <v>43</v>
       </c>
-      <c r="AI12" t="s">
+      <c r="AJ12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -2184,7 +2255,7 @@
         <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" t="s">
         <v>53</v>
@@ -2196,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H13">
         <v>5</v>
@@ -2217,13 +2288,13 @@
         <v>16</v>
       </c>
       <c r="N13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O13">
         <v>8</v>
       </c>
       <c r="P13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q13">
         <v>5</v>
@@ -2231,59 +2302,62 @@
       <c r="R13">
         <v>13843</v>
       </c>
-      <c r="S13">
+      <c r="S13" t="s">
+        <v>8</v>
+      </c>
+      <c r="T13">
         <v>32768</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>35</v>
       </c>
-      <c r="U13" s="1">
+      <c r="V13" s="1">
         <v>125</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>1169</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>414</v>
       </c>
-      <c r="X13" s="1">
+      <c r="Y13" s="1">
         <v>80</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>416</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>176</v>
       </c>
-      <c r="AA13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB13" s="1">
-        <v>8</v>
-      </c>
-      <c r="AC13">
+      <c r="AB13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>8</v>
+      </c>
+      <c r="AD13">
         <v>376</v>
       </c>
-      <c r="AD13">
+      <c r="AE13">
         <v>104</v>
       </c>
-      <c r="AE13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF13" s="1" t="s">
+      <c r="AF13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AG13" t="s">
+      <c r="AH13" t="s">
         <v>31</v>
       </c>
-      <c r="AH13" t="s">
-        <v>8</v>
-      </c>
       <c r="AI13" t="s">
         <v>8</v>
       </c>
+      <c r="AJ13" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -2291,7 +2365,7 @@
         <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D14" t="s">
         <v>53</v>
@@ -2303,7 +2377,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H14">
         <v>5</v>
@@ -2324,13 +2398,13 @@
         <v>16</v>
       </c>
       <c r="N14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O14">
         <v>8</v>
       </c>
       <c r="P14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q14">
         <v>5</v>
@@ -2338,59 +2412,62 @@
       <c r="R14">
         <v>13843</v>
       </c>
-      <c r="S14">
+      <c r="S14" t="s">
+        <v>8</v>
+      </c>
+      <c r="T14">
         <v>32768</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>35</v>
       </c>
-      <c r="U14" s="1">
+      <c r="V14" s="1">
         <v>125</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>1169</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>414</v>
       </c>
-      <c r="X14" s="1">
+      <c r="Y14" s="1">
         <v>80</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>416</v>
       </c>
-      <c r="Z14">
+      <c r="AA14">
         <v>176</v>
       </c>
-      <c r="AA14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB14" s="1">
+      <c r="AB14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC14" s="1">
         <v>16</v>
       </c>
-      <c r="AC14">
+      <c r="AD14">
         <v>368</v>
       </c>
-      <c r="AD14">
+      <c r="AE14">
         <v>112</v>
       </c>
-      <c r="AE14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF14" s="1" t="s">
+      <c r="AF14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AG14" t="s">
+      <c r="AH14" t="s">
         <v>51</v>
       </c>
-      <c r="AH14" t="s">
-        <v>8</v>
-      </c>
       <c r="AI14" t="s">
         <v>8</v>
       </c>
+      <c r="AJ14" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="15" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>54</v>
       </c>
@@ -2398,7 +2475,7 @@
         <v>68</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>72</v>
@@ -2410,7 +2487,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H15" s="4">
         <v>5</v>
@@ -2431,13 +2508,13 @@
         <v>16</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O15" s="4">
         <v>8</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q15" s="10">
         <v>10</v>
@@ -2445,59 +2522,62 @@
       <c r="R15" s="4">
         <v>10135</v>
       </c>
-      <c r="S15" s="4">
+      <c r="S15" t="s">
+        <v>8</v>
+      </c>
+      <c r="T15" s="4">
         <v>32768</v>
       </c>
-      <c r="T15" s="4" t="s">
+      <c r="U15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="U15" s="5">
+      <c r="V15" s="5">
         <v>125</v>
       </c>
-      <c r="V15" s="4">
+      <c r="W15" s="4">
         <v>1169</v>
       </c>
-      <c r="W15" s="4">
+      <c r="X15" s="4">
         <v>414</v>
       </c>
-      <c r="X15" s="5">
+      <c r="Y15" s="5">
         <v>64</v>
       </c>
-      <c r="Y15" s="4">
+      <c r="Z15" s="4">
         <v>400</v>
       </c>
-      <c r="Z15" s="4">
+      <c r="AA15" s="4">
         <v>160</v>
       </c>
-      <c r="AA15" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB15" s="9">
-        <v>8</v>
-      </c>
-      <c r="AC15" s="4">
+      <c r="AB15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC15" s="9">
+        <v>8</v>
+      </c>
+      <c r="AD15" s="4">
         <v>368</v>
       </c>
-      <c r="AD15" s="4">
+      <c r="AE15" s="4">
         <v>96</v>
       </c>
-      <c r="AE15" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF15" s="5" t="s">
+      <c r="AF15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG15" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AG15" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH15" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI15" s="15" t="s">
+      <c r="AH15" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ15" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -2505,7 +2585,7 @@
         <v>68</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D16" t="s">
         <v>53</v>
@@ -2517,7 +2597,7 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H16">
         <v>5</v>
@@ -2538,13 +2618,13 @@
         <v>16</v>
       </c>
       <c r="N16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O16">
         <v>8</v>
       </c>
       <c r="P16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q16">
         <v>5</v>
@@ -2552,59 +2632,62 @@
       <c r="R16">
         <v>10135</v>
       </c>
-      <c r="S16">
+      <c r="S16" t="s">
+        <v>8</v>
+      </c>
+      <c r="T16">
         <v>32768</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>35</v>
       </c>
-      <c r="U16" s="1">
+      <c r="V16" s="1">
         <v>125</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>1169</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>414</v>
       </c>
-      <c r="X16" s="1">
+      <c r="Y16" s="1">
         <v>64</v>
       </c>
-      <c r="Y16">
+      <c r="Z16">
         <v>400</v>
       </c>
-      <c r="Z16">
+      <c r="AA16">
         <v>160</v>
       </c>
-      <c r="AA16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB16" s="1">
+      <c r="AB16" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC16" s="1">
         <v>24</v>
       </c>
-      <c r="AC16">
+      <c r="AD16">
         <v>384</v>
       </c>
-      <c r="AD16">
+      <c r="AE16">
         <v>120</v>
       </c>
-      <c r="AE16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF16" s="1" t="s">
+      <c r="AF16" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AG16" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH16" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI16" s="14" t="s">
+      <c r="AH16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -2612,7 +2695,7 @@
         <v>69</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D17" t="s">
         <v>53</v>
@@ -2624,7 +2707,7 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H17">
         <v>5</v>
@@ -2645,13 +2728,13 @@
         <v>16</v>
       </c>
       <c r="N17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O17">
         <v>8</v>
       </c>
       <c r="P17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q17">
         <v>5</v>
@@ -2659,59 +2742,62 @@
       <c r="R17">
         <v>10999</v>
       </c>
-      <c r="S17">
+      <c r="S17" t="s">
+        <v>8</v>
+      </c>
+      <c r="T17">
         <v>32768</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>35</v>
       </c>
-      <c r="U17" s="1">
+      <c r="V17" s="1">
         <v>125</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>1169</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>414</v>
       </c>
-      <c r="X17" s="1">
+      <c r="Y17" s="1">
         <v>64</v>
       </c>
-      <c r="Y17">
+      <c r="Z17">
         <v>400</v>
       </c>
-      <c r="Z17">
+      <c r="AA17">
         <v>176</v>
       </c>
-      <c r="AA17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB17" s="1">
+      <c r="AB17" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC17" s="1">
         <v>24</v>
       </c>
-      <c r="AC17">
+      <c r="AD17">
         <v>384</v>
       </c>
-      <c r="AD17">
+      <c r="AE17">
         <v>112</v>
       </c>
-      <c r="AE17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF17" s="1" t="s">
+      <c r="AF17" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AG17" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH17" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI17" s="14" t="s">
+      <c r="AH17" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -2719,7 +2805,7 @@
         <v>69</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" t="s">
         <v>53</v>
@@ -2731,7 +2817,7 @@
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H18">
         <v>5</v>
@@ -2752,13 +2838,13 @@
         <v>16</v>
       </c>
       <c r="N18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O18">
         <v>8</v>
       </c>
       <c r="P18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q18">
         <v>5</v>
@@ -2766,59 +2852,62 @@
       <c r="R18">
         <v>11843</v>
       </c>
-      <c r="S18">
+      <c r="S18" t="s">
+        <v>8</v>
+      </c>
+      <c r="T18">
         <v>32768</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>35</v>
       </c>
-      <c r="U18" s="1">
+      <c r="V18" s="1">
         <v>125</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <v>1169</v>
       </c>
-      <c r="W18">
+      <c r="X18">
         <v>414</v>
       </c>
-      <c r="X18" s="1">
+      <c r="Y18" s="1">
         <v>64</v>
       </c>
-      <c r="Y18">
+      <c r="Z18">
         <v>400</v>
       </c>
-      <c r="Z18">
+      <c r="AA18">
         <v>192</v>
       </c>
-      <c r="AA18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB18" s="1">
+      <c r="AB18" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC18" s="1">
         <v>24</v>
       </c>
-      <c r="AC18">
+      <c r="AD18">
         <v>384</v>
       </c>
-      <c r="AD18">
+      <c r="AE18">
         <v>104</v>
       </c>
-      <c r="AE18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF18" s="1" t="s">
+      <c r="AF18" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AG18" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH18" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI18" s="14" t="s">
+      <c r="AH18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -2826,7 +2915,7 @@
         <v>70</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19" t="s">
         <v>53</v>
@@ -2838,7 +2927,7 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H19">
         <v>5</v>
@@ -2859,13 +2948,13 @@
         <v>16</v>
       </c>
       <c r="N19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O19">
         <v>8</v>
       </c>
       <c r="P19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q19">
         <v>5</v>
@@ -2873,59 +2962,62 @@
       <c r="R19">
         <v>10473</v>
       </c>
-      <c r="S19">
+      <c r="S19" t="s">
+        <v>8</v>
+      </c>
+      <c r="T19">
         <v>32768</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
         <v>35</v>
       </c>
-      <c r="U19" s="1">
+      <c r="V19" s="1">
         <v>125</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>1169</v>
       </c>
-      <c r="W19">
+      <c r="X19">
         <v>414</v>
       </c>
-      <c r="X19" s="1">
+      <c r="Y19" s="1">
         <v>64</v>
       </c>
-      <c r="Y19">
+      <c r="Z19">
         <v>416</v>
       </c>
-      <c r="Z19">
+      <c r="AA19">
         <v>160</v>
       </c>
-      <c r="AA19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB19" s="1">
+      <c r="AB19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC19" s="1">
         <v>24</v>
       </c>
-      <c r="AC19">
+      <c r="AD19">
         <v>376</v>
       </c>
-      <c r="AD19">
+      <c r="AE19">
         <v>120</v>
       </c>
-      <c r="AE19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF19" s="1" t="s">
+      <c r="AF19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AG19" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH19" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI19" s="14" t="s">
+      <c r="AH19" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -2933,7 +3025,7 @@
         <v>70</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
         <v>53</v>
@@ -2945,7 +3037,7 @@
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H20">
         <v>5</v>
@@ -2966,13 +3058,13 @@
         <v>16</v>
       </c>
       <c r="N20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O20">
         <v>8</v>
       </c>
       <c r="P20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q20">
         <v>5</v>
@@ -2980,59 +3072,62 @@
       <c r="R20">
         <v>10825</v>
       </c>
-      <c r="S20">
+      <c r="S20" t="s">
+        <v>8</v>
+      </c>
+      <c r="T20">
         <v>32768</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
         <v>35</v>
       </c>
-      <c r="U20" s="1">
+      <c r="V20" s="1">
         <v>125</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>1169</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>414</v>
       </c>
-      <c r="X20" s="1">
+      <c r="Y20" s="1">
         <v>64</v>
       </c>
-      <c r="Y20">
+      <c r="Z20">
         <v>432</v>
       </c>
-      <c r="Z20">
+      <c r="AA20">
         <v>160</v>
       </c>
-      <c r="AA20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB20" s="1">
+      <c r="AB20" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC20" s="1">
         <v>24</v>
       </c>
-      <c r="AC20">
+      <c r="AD20">
         <v>368</v>
       </c>
-      <c r="AD20">
+      <c r="AE20">
         <v>120</v>
       </c>
-      <c r="AE20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF20" s="1" t="s">
+      <c r="AF20" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG20" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AG20" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH20" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI20" s="14" t="s">
+      <c r="AH20" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -3040,7 +3135,7 @@
         <v>71</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D21" t="s">
         <v>53</v>
@@ -3052,7 +3147,7 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H21">
         <v>5</v>
@@ -3073,13 +3168,13 @@
         <v>16</v>
       </c>
       <c r="N21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O21">
         <v>8</v>
       </c>
       <c r="P21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q21">
         <v>5</v>
@@ -3087,59 +3182,62 @@
       <c r="R21">
         <v>12317</v>
       </c>
-      <c r="S21">
+      <c r="S21" t="s">
+        <v>8</v>
+      </c>
+      <c r="T21">
         <v>32768</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>35</v>
       </c>
-      <c r="U21" s="1">
+      <c r="V21" s="1">
         <v>125</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>1169</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <v>414</v>
       </c>
-      <c r="X21" s="1">
+      <c r="Y21" s="1">
         <v>80</v>
       </c>
-      <c r="Y21">
+      <c r="Z21">
         <v>400</v>
       </c>
-      <c r="Z21">
+      <c r="AA21">
         <v>160</v>
       </c>
-      <c r="AA21" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB21" s="1">
+      <c r="AB21" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC21" s="1">
         <v>16</v>
       </c>
-      <c r="AC21">
+      <c r="AD21">
         <v>384</v>
       </c>
-      <c r="AD21">
+      <c r="AE21">
         <v>120</v>
       </c>
-      <c r="AE21" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF21" s="1" t="s">
+      <c r="AF21" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AG21" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH21" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI21" s="14" t="s">
+      <c r="AH21" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -3147,7 +3245,7 @@
         <v>71</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D22" t="s">
         <v>53</v>
@@ -3159,7 +3257,7 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H22">
         <v>5</v>
@@ -3180,13 +3278,13 @@
         <v>16</v>
       </c>
       <c r="N22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O22">
         <v>8</v>
       </c>
       <c r="P22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q22">
         <v>5</v>
@@ -3194,271 +3292,511 @@
       <c r="R22">
         <v>14443</v>
       </c>
-      <c r="S22">
+      <c r="S22" t="s">
+        <v>8</v>
+      </c>
+      <c r="T22">
         <v>32768</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>35</v>
       </c>
-      <c r="U22" s="1">
+      <c r="V22" s="1">
         <v>125</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>1169</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>414</v>
       </c>
-      <c r="X22" s="1">
+      <c r="Y22" s="1">
         <v>96</v>
       </c>
-      <c r="Y22">
+      <c r="Z22">
         <v>400</v>
       </c>
-      <c r="Z22">
+      <c r="AA22">
         <v>160</v>
       </c>
-      <c r="AA22" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB22" s="1">
-        <v>8</v>
-      </c>
-      <c r="AC22">
+      <c r="AB22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>8</v>
+      </c>
+      <c r="AD22">
         <v>384</v>
       </c>
-      <c r="AD22">
+      <c r="AE22">
         <v>120</v>
       </c>
-      <c r="AE22" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF22" s="1" t="s">
+      <c r="AF22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG22" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AG22" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH22" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI22" s="14" t="s">
+      <c r="AH22" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="L23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="M23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="N23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="O23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="P23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="R23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="S23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="T23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="U23" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="V23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="W23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="X23" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB23" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF23" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI23" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M23" t="s">
+        <v>8</v>
+      </c>
+      <c r="N23" t="s">
+        <v>8</v>
+      </c>
+      <c r="O23" t="s">
+        <v>8</v>
+      </c>
+      <c r="P23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>8</v>
+      </c>
+      <c r="R23" t="s">
+        <v>8</v>
+      </c>
+      <c r="S23" t="s">
+        <v>8</v>
+      </c>
+      <c r="T23" t="s">
+        <v>8</v>
+      </c>
+      <c r="U23" t="s">
+        <v>8</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="W23" t="s">
+        <v>8</v>
+      </c>
+      <c r="X23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>114</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="24" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="L24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="M24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="N24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="O24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="P24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="R24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="S24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="T24" s="14" t="s">
+      <c r="D24" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="P24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="R24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="S24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="T24" s="16" t="s">
         <v>8</v>
       </c>
       <c r="U24" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="V24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="W24" s="14" t="s">
+      <c r="V24" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="W24" s="16" t="s">
         <v>8</v>
       </c>
       <c r="X24" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="Y24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA24" s="14" t="s">
+      <c r="Y24" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA24" s="16" t="s">
         <v>8</v>
       </c>
       <c r="AB24" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="AC24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE24" s="14" t="s">
+      <c r="AC24" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE24" s="16" t="s">
         <v>8</v>
       </c>
       <c r="AF24" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="AG24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI24" s="14" t="s">
-        <v>8</v>
-      </c>
+      <c r="AG24" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ24" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="15">
+        <v>5</v>
+      </c>
+      <c r="I25" s="15">
+        <v>3</v>
+      </c>
+      <c r="J25" s="15">
+        <v>2</v>
+      </c>
+      <c r="K25" s="15">
+        <v>3</v>
+      </c>
+      <c r="L25" s="15">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>16</v>
+      </c>
+      <c r="N25" t="s">
+        <v>107</v>
+      </c>
+      <c r="O25">
+        <v>8</v>
+      </c>
+      <c r="P25" t="s">
+        <v>109</v>
+      </c>
+      <c r="S25" s="14">
+        <f t="shared" ref="S25" si="0" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (Y25*Z25*AA25)</f>
+        <v>83027.753778838392</v>
+      </c>
+      <c r="T25" s="14">
+        <v>81920</v>
+      </c>
+      <c r="U25" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="V25" s="1">
+        <v>125</v>
+      </c>
+      <c r="W25" s="14">
+        <v>1169</v>
+      </c>
+      <c r="X25" s="14">
+        <v>414</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>112</v>
+      </c>
+      <c r="Z25" s="14">
+        <v>864</v>
+      </c>
+      <c r="AA25" s="14">
+        <v>400</v>
+      </c>
+      <c r="AB25" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC25" s="1">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((V25 - Y25) / 2)</f>
+        <v>6</v>
+      </c>
+      <c r="AD25" s="14">
+        <f t="shared" ref="AD25" si="1" xml:space="preserve"> _xlfn.FLOOR.MATH((W25 - Z25) / 2)</f>
+        <v>152</v>
+      </c>
+      <c r="AE25" s="14">
+        <f t="shared" ref="AE25" si="2" xml:space="preserve"> _xlfn.FLOOR.MATH((X25 - AA25) / 2)</f>
+        <v>7</v>
+      </c>
+      <c r="AF25" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="15">
+        <v>5</v>
+      </c>
+      <c r="I26" s="15">
+        <v>3</v>
+      </c>
+      <c r="J26" s="15">
+        <v>2</v>
+      </c>
+      <c r="K26" s="15">
+        <v>3</v>
+      </c>
+      <c r="L26" s="15">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>16</v>
+      </c>
+      <c r="N26" t="s">
+        <v>107</v>
+      </c>
+      <c r="O26">
+        <v>8</v>
+      </c>
+      <c r="P26" t="s">
+        <v>109</v>
+      </c>
+      <c r="S26" s="14">
+        <f t="shared" ref="S26" si="3" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (Y26*Z26*AA26)</f>
+        <v>81518.129922434266</v>
+      </c>
+      <c r="T26" s="14">
+        <v>81920</v>
+      </c>
+      <c r="U26" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="V26" s="1">
+        <v>125</v>
+      </c>
+      <c r="W26" s="14">
+        <v>1169</v>
+      </c>
+      <c r="X26" s="14">
+        <v>414</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>112</v>
+      </c>
+      <c r="Z26" s="14">
+        <v>848</v>
+      </c>
+      <c r="AA26" s="14">
+        <v>400</v>
+      </c>
+      <c r="AB26" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC26" s="1">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((V26 - Y26) / 2)</f>
+        <v>6</v>
+      </c>
+      <c r="AD26" s="14">
+        <f t="shared" ref="AD26" si="4" xml:space="preserve"> _xlfn.FLOOR.MATH((W26 - Z26) / 2)</f>
+        <v>160</v>
+      </c>
+      <c r="AE26" s="14">
+        <f t="shared" ref="AE26" si="5" xml:space="preserve"> _xlfn.FLOOR.MATH((X26 - AA26) / 2)</f>
+        <v>7</v>
+      </c>
+      <c r="AF26" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S28" s="14"/>
+      <c r="T28" s="14"/>
+      <c r="U28" s="14"/>
+      <c r="W28" s="14"/>
+      <c r="X28" s="14"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="14"/>
+      <c r="AB28" s="14"/>
+      <c r="AD28" s="14"/>
+      <c r="AE28" s="14"/>
+      <c r="AF28" s="14"/>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="Z29" s="14"/>
+      <c r="AA29" s="14"/>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="Z30" s="14"/>
+      <c r="AA30" s="14"/>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="Z31" s="14"/>
+      <c r="AA31" s="14"/>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="Z32" s="14"/>
+      <c r="AA32" s="14"/>
+    </row>
+    <row r="33" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z33" s="14"/>
+      <c r="AA33" s="14"/>
+    </row>
+    <row r="34" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z34" s="14"/>
+      <c r="AA34" s="14"/>
+    </row>
+    <row r="35" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z35" s="14"/>
+      <c r="AA35" s="14"/>
+    </row>
+    <row r="36" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z36" s="14"/>
+      <c r="AA36" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
add 3 sessions to VRAM table, a100 dataset03 runs
</commit_message>
<xml_diff>
--- a/VRAM patch stride table.xlsx
+++ b/VRAM patch stride table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE641904-7DF7-4885-8F40-BD67E4228A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E5278A-0B65-445F-A7CD-8E1F109E4141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="140">
   <si>
     <t>patch z</t>
   </si>
@@ -159,15 +159,9 @@
     <t>session</t>
   </si>
   <si>
-    <t>VRAM capacity (MiB)</t>
-  </si>
-  <si>
     <t>GPU</t>
   </si>
   <si>
-    <t>VRAM usage (MiB)</t>
-  </si>
-  <si>
     <t>ValueError: requested an output size of torch.Size([9, 21, 51]), but valid sizes range from [7, 19, 49] to [8, 20, 50] (for an input of torch.Size([4, 10, 25]))</t>
   </si>
   <si>
@@ -415,6 +409,54 @@
   </si>
   <si>
     <t>stride = foor (resolution - patch) / 2</t>
+  </si>
+  <si>
+    <t>TBD copy</t>
+  </si>
+  <si>
+    <t>torch.cuda.OutOfMemoryError: CUDA out of memory. Tried to allocate 4.53 GiB (GPU 0; 79.15 GiB total capacity; 68.20 GiB already allocated; 1.93 GiB free; 75.58 GiB reserved in total by PyTorch) If reserved memory is &gt;&gt; allocated memory try setting max_split_size_mb to avoid fragmentation.  See documentation for Memory Management and PYTORCH_CUDA_ALLOC_CONF</t>
+  </si>
+  <si>
+    <t>File "/home/dwalth/data/conda/envs/3dunet/lib/python3.11/site-packages/torch/autograd/__init__.py", line 200, in backward: Variable._execution_engine.run_backward(  # Calls into the C++ engine to run the backward pass</t>
+  </si>
+  <si>
+    <t>VRAM capactiy (GiB) from cuda error messages</t>
+  </si>
+  <si>
+    <t>VRAM capacity (MiB, converted from GiB) from cuda error messages</t>
+  </si>
+  <si>
+    <t>VRAM usage (GiB) from cuda error messages</t>
+  </si>
+  <si>
+    <t>VRAM usage (MiB) nvidia-smi output</t>
+  </si>
+  <si>
+    <t>VRAM capacity (MiB) nvidia-smi output</t>
+  </si>
+  <si>
+    <t>VRAM usage (MiB, converted from GiB) from cuda error messages</t>
+  </si>
+  <si>
+    <t>patch = arbitrary even int_2^4</t>
+  </si>
+  <si>
+    <t>stride = foor (resolution - patch) / 3</t>
+  </si>
+  <si>
+    <t>230905-2</t>
+  </si>
+  <si>
+    <t>no, but ended prematurely</t>
+  </si>
+  <si>
+    <t>no, more VRAM required than expected, i.e., predicted</t>
+  </si>
+  <si>
+    <t>fit VRAM on A100 to get better performance metrics</t>
+  </si>
+  <si>
+    <t>expect VRAM ~ patch volume + overhead (few GiBs)</t>
   </si>
 </sst>
 </file>
@@ -550,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -567,10 +609,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:AO36"/>
+  <dimension ref="A1:AS27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -904,151 +945,163 @@
     <col min="14" max="14" width="8.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="15" max="16" width="5.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="17" max="17" width="9.140625" collapsed="1"/>
-    <col min="18" max="19" width="9.140625" customWidth="1"/>
-    <col min="20" max="20" width="7.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="23.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="6" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.28515625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" customWidth="1"/>
-    <col min="27" max="28" width="5" customWidth="1"/>
-    <col min="29" max="29" width="6.140625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="6.5703125" customWidth="1"/>
-    <col min="31" max="31" width="5" customWidth="1"/>
-    <col min="32" max="32" width="6" customWidth="1"/>
-    <col min="33" max="33" width="34.28515625" style="1" customWidth="1"/>
-    <col min="34" max="34" width="131.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="47" customWidth="1"/>
-    <col min="37" max="37" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="41" max="41" width="12.140625" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="21" width="9.140625" customWidth="1"/>
+    <col min="22" max="24" width="7.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="23.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.28515625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="6.140625" customWidth="1"/>
+    <col min="31" max="32" width="5" customWidth="1"/>
+    <col min="33" max="33" width="6.140625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="6.5703125" customWidth="1"/>
+    <col min="35" max="35" width="5" customWidth="1"/>
+    <col min="36" max="36" width="6" customWidth="1"/>
+    <col min="37" max="37" width="34.28515625" style="1" customWidth="1"/>
+    <col min="38" max="38" width="131.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="47" customWidth="1"/>
+    <col min="41" max="41" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.140625" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="P1" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AF1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AD1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>58</v>
       </c>
-      <c r="AG1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>60</v>
-      </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1057,7 +1110,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H2">
         <v>5</v>
@@ -1078,13 +1131,13 @@
         <v>16</v>
       </c>
       <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
         <v>107</v>
-      </c>
-      <c r="O2">
-        <v>8</v>
-      </c>
-      <c r="P2" t="s">
-        <v>109</v>
       </c>
       <c r="Q2">
         <v>5</v>
@@ -1095,70 +1148,82 @@
       <c r="S2" t="s">
         <v>8</v>
       </c>
-      <c r="T2">
+      <c r="T2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2">
         <v>32768</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y2" t="s">
         <v>35</v>
       </c>
-      <c r="V2" s="1">
+      <c r="Z2" s="1">
         <v>125</v>
       </c>
-      <c r="W2">
+      <c r="AA2">
         <v>1169</v>
       </c>
-      <c r="X2">
+      <c r="AB2">
         <v>414</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="AC2" s="1">
         <v>105</v>
       </c>
-      <c r="Z2">
+      <c r="AD2">
         <v>1149</v>
       </c>
-      <c r="AA2">
+      <c r="AE2">
         <v>394</v>
       </c>
-      <c r="AB2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC2" s="1">
+      <c r="AF2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG2" s="1">
         <v>10</v>
       </c>
-      <c r="AD2">
+      <c r="AH2">
         <v>10</v>
       </c>
-      <c r="AE2">
+      <c r="AI2">
         <v>10</v>
       </c>
-      <c r="AF2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AJ2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AL2" t="s">
         <v>16</v>
       </c>
-      <c r="AI2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="AM2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1167,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H3">
         <v>5</v>
@@ -1188,13 +1253,13 @@
         <v>16</v>
       </c>
       <c r="N3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O3">
+        <v>8</v>
+      </c>
+      <c r="P3" t="s">
         <v>107</v>
-      </c>
-      <c r="O3">
-        <v>8</v>
-      </c>
-      <c r="P3" t="s">
-        <v>109</v>
       </c>
       <c r="Q3">
         <v>10</v>
@@ -1205,70 +1270,82 @@
       <c r="S3" t="s">
         <v>8</v>
       </c>
-      <c r="T3">
+      <c r="T3" t="s">
+        <v>8</v>
+      </c>
+      <c r="U3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3">
         <v>32768</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y3" t="s">
         <v>35</v>
       </c>
-      <c r="V3" s="1">
+      <c r="Z3" s="1">
         <v>125</v>
       </c>
-      <c r="W3">
+      <c r="AA3">
         <v>1169</v>
       </c>
-      <c r="X3">
+      <c r="AB3">
         <v>414</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="AC3" s="1">
         <v>100</v>
       </c>
-      <c r="Z3">
+      <c r="AD3">
         <v>1100</v>
       </c>
-      <c r="AA3">
+      <c r="AE3">
         <v>390</v>
       </c>
-      <c r="AB3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC3" s="1">
+      <c r="AF3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG3" s="1">
         <v>10</v>
       </c>
-      <c r="AD3">
+      <c r="AH3">
         <v>10</v>
       </c>
-      <c r="AE3">
+      <c r="AI3">
         <v>10</v>
       </c>
-      <c r="AF3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AJ3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AL3" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ3" t="s">
+      <c r="AM3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
         <v>94</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>96</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1277,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -1298,14 +1375,14 @@
         <v>16</v>
       </c>
       <c r="N4" t="s">
+        <v>105</v>
+      </c>
+      <c r="O4">
+        <v>8</v>
+      </c>
+      <c r="P4" t="s">
         <v>107</v>
       </c>
-      <c r="O4">
-        <v>8</v>
-      </c>
-      <c r="P4" t="s">
-        <v>109</v>
-      </c>
       <c r="Q4" t="s">
         <v>8</v>
       </c>
@@ -1315,70 +1392,82 @@
       <c r="S4" t="s">
         <v>8</v>
       </c>
-      <c r="T4">
+      <c r="T4" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4">
         <v>32768</v>
       </c>
-      <c r="U4" t="s">
+      <c r="W4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y4" t="s">
         <v>35</v>
       </c>
-      <c r="V4" s="1">
+      <c r="Z4" s="1">
         <v>125</v>
       </c>
-      <c r="W4">
+      <c r="AA4">
         <v>1169</v>
       </c>
-      <c r="X4">
+      <c r="AB4">
         <v>414</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="AC4" s="1">
         <v>100</v>
       </c>
-      <c r="Z4">
+      <c r="AD4">
         <v>1100</v>
       </c>
-      <c r="AA4">
+      <c r="AE4">
         <v>390</v>
       </c>
-      <c r="AB4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC4" s="1">
+      <c r="AF4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG4" s="1">
         <v>26</v>
       </c>
-      <c r="AD4">
+      <c r="AH4">
         <v>70</v>
       </c>
-      <c r="AE4">
+      <c r="AI4">
         <v>25</v>
       </c>
-      <c r="AF4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AJ4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AL4" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AM4" t="s">
         <v>15</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AN4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1387,7 +1476,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H5">
         <v>5</v>
@@ -1408,14 +1497,14 @@
         <v>16</v>
       </c>
       <c r="N5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O5">
+        <v>8</v>
+      </c>
+      <c r="P5" t="s">
         <v>107</v>
       </c>
-      <c r="O5">
-        <v>8</v>
-      </c>
-      <c r="P5" t="s">
-        <v>109</v>
-      </c>
       <c r="Q5" t="s">
         <v>8</v>
       </c>
@@ -1425,70 +1514,82 @@
       <c r="S5" t="s">
         <v>8</v>
       </c>
-      <c r="T5">
+      <c r="T5" t="s">
+        <v>8</v>
+      </c>
+      <c r="U5" t="s">
+        <v>8</v>
+      </c>
+      <c r="V5">
         <v>32768</v>
       </c>
-      <c r="U5" t="s">
+      <c r="W5" t="s">
+        <v>8</v>
+      </c>
+      <c r="X5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y5" t="s">
         <v>35</v>
       </c>
-      <c r="V5" s="1">
+      <c r="Z5" s="1">
         <v>125</v>
       </c>
-      <c r="W5">
+      <c r="AA5">
         <v>1169</v>
       </c>
-      <c r="X5">
+      <c r="AB5">
         <v>414</v>
       </c>
-      <c r="Y5" s="1">
+      <c r="AC5" s="1">
         <v>100</v>
       </c>
-      <c r="Z5">
+      <c r="AD5">
         <v>1100</v>
       </c>
-      <c r="AA5">
+      <c r="AE5">
         <v>390</v>
       </c>
-      <c r="AB5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC5" s="1">
+      <c r="AF5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG5" s="1">
         <v>25</v>
       </c>
-      <c r="AD5">
+      <c r="AH5">
         <v>69</v>
       </c>
-      <c r="AE5">
+      <c r="AI5">
         <v>24</v>
       </c>
-      <c r="AF5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG5" s="1" t="s">
+      <c r="AJ5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AL5" t="s">
         <v>9</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AM5" t="s">
         <v>15</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AN5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1497,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -1518,13 +1619,13 @@
         <v>16</v>
       </c>
       <c r="N6" t="s">
+        <v>105</v>
+      </c>
+      <c r="O6">
+        <v>8</v>
+      </c>
+      <c r="P6" t="s">
         <v>107</v>
-      </c>
-      <c r="O6">
-        <v>8</v>
-      </c>
-      <c r="P6" t="s">
-        <v>109</v>
       </c>
       <c r="Q6">
         <v>5</v>
@@ -1535,64 +1636,76 @@
       <c r="S6" t="s">
         <v>8</v>
       </c>
-      <c r="T6">
+      <c r="T6" t="s">
+        <v>8</v>
+      </c>
+      <c r="U6" t="s">
+        <v>8</v>
+      </c>
+      <c r="V6">
         <v>32768</v>
       </c>
-      <c r="U6" t="s">
+      <c r="W6" t="s">
+        <v>8</v>
+      </c>
+      <c r="X6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y6" t="s">
         <v>35</v>
       </c>
-      <c r="V6" s="1">
+      <c r="Z6" s="1">
         <v>125</v>
       </c>
-      <c r="W6">
+      <c r="AA6">
         <v>1169</v>
       </c>
-      <c r="X6">
+      <c r="AB6">
         <v>414</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="AC6" s="1">
         <v>101</v>
       </c>
-      <c r="Z6">
+      <c r="AD6">
         <v>1009</v>
       </c>
-      <c r="AA6">
+      <c r="AE6">
         <v>400</v>
       </c>
-      <c r="AB6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC6" s="1">
+      <c r="AF6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG6" s="1">
         <v>12</v>
       </c>
-      <c r="AD6">
+      <c r="AH6">
         <v>90</v>
       </c>
-      <c r="AE6">
+      <c r="AI6">
         <v>7</v>
       </c>
-      <c r="AF6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG6" s="1" t="s">
+      <c r="AJ6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AL6" t="s">
         <v>16</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AM6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1601,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H7">
         <v>5</v>
@@ -1622,14 +1735,14 @@
         <v>16</v>
       </c>
       <c r="N7" t="s">
+        <v>105</v>
+      </c>
+      <c r="O7">
+        <v>8</v>
+      </c>
+      <c r="P7" t="s">
         <v>107</v>
       </c>
-      <c r="O7">
-        <v>8</v>
-      </c>
-      <c r="P7" t="s">
-        <v>109</v>
-      </c>
       <c r="Q7">
         <v>5</v>
       </c>
@@ -1639,76 +1752,88 @@
       <c r="S7" t="s">
         <v>8</v>
       </c>
-      <c r="T7">
+      <c r="T7" t="s">
+        <v>8</v>
+      </c>
+      <c r="U7" t="s">
+        <v>8</v>
+      </c>
+      <c r="V7">
         <v>32768</v>
       </c>
-      <c r="U7" t="s">
+      <c r="W7" t="s">
+        <v>8</v>
+      </c>
+      <c r="X7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y7" t="s">
         <v>35</v>
       </c>
-      <c r="V7" s="1">
+      <c r="Z7" s="1">
         <v>125</v>
       </c>
-      <c r="W7">
+      <c r="AA7">
         <v>1169</v>
       </c>
-      <c r="X7">
+      <c r="AB7">
         <v>414</v>
       </c>
-      <c r="Y7" s="1">
-        <f>V7-50</f>
+      <c r="AC7" s="1">
+        <f>Z7-50</f>
         <v>75</v>
       </c>
-      <c r="Z7">
-        <f>W7-240</f>
+      <c r="AD7">
+        <f>AA7-240</f>
         <v>929</v>
       </c>
-      <c r="AA7">
-        <f>X7-110</f>
+      <c r="AE7">
+        <f>AB7-110</f>
         <v>304</v>
       </c>
-      <c r="AB7" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC7" s="6">
-        <f>(V7-Y7)/2</f>
+      <c r="AF7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG7" s="6">
+        <f>(Z7-AC7)/2</f>
         <v>25</v>
       </c>
-      <c r="AD7" s="7">
-        <f>(W7-Z7)/2</f>
+      <c r="AH7" s="7">
+        <f>(AA7-AD7)/2</f>
         <v>120</v>
       </c>
-      <c r="AE7" s="7">
-        <f>(X7-AA7)/2</f>
+      <c r="AI7" s="7">
+        <f>(AB7-AE7)/2</f>
         <v>55</v>
       </c>
-      <c r="AF7" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG7" s="1" t="s">
+      <c r="AJ7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AL7" t="s">
         <v>16</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AM7" t="s">
         <v>26</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AN7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1717,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H8">
         <v>5</v>
@@ -1738,14 +1863,14 @@
         <v>16</v>
       </c>
       <c r="N8" t="s">
+        <v>105</v>
+      </c>
+      <c r="O8">
+        <v>8</v>
+      </c>
+      <c r="P8" t="s">
         <v>107</v>
       </c>
-      <c r="O8">
-        <v>8</v>
-      </c>
-      <c r="P8" t="s">
-        <v>109</v>
-      </c>
       <c r="Q8">
         <v>5</v>
       </c>
@@ -1755,70 +1880,82 @@
       <c r="S8" t="s">
         <v>8</v>
       </c>
-      <c r="T8">
+      <c r="T8" t="s">
+        <v>8</v>
+      </c>
+      <c r="U8" t="s">
+        <v>8</v>
+      </c>
+      <c r="V8">
         <v>32768</v>
       </c>
-      <c r="U8" t="s">
+      <c r="W8" t="s">
+        <v>8</v>
+      </c>
+      <c r="X8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y8" t="s">
         <v>35</v>
       </c>
-      <c r="V8" s="1">
+      <c r="Z8" s="1">
         <v>125</v>
       </c>
-      <c r="W8">
+      <c r="AA8">
         <v>1169</v>
       </c>
-      <c r="X8">
+      <c r="AB8">
         <v>414</v>
       </c>
-      <c r="Y8" s="1">
+      <c r="AC8" s="1">
         <v>72</v>
       </c>
-      <c r="Z8">
+      <c r="AD8">
         <v>928</v>
       </c>
-      <c r="AA8">
+      <c r="AE8">
         <v>304</v>
       </c>
-      <c r="AB8" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC8" s="1">
+      <c r="AF8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG8" s="1">
         <v>24</v>
       </c>
-      <c r="AD8">
+      <c r="AH8">
         <v>120</v>
       </c>
-      <c r="AE8">
+      <c r="AI8">
         <v>48</v>
       </c>
-      <c r="AF8" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG8" s="1" t="s">
+      <c r="AJ8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AI8" t="s">
+      <c r="AL8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM8" t="s">
         <v>26</v>
       </c>
-      <c r="AJ8" t="s">
+      <c r="AN8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1827,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H9">
         <v>5</v>
@@ -1848,13 +1985,13 @@
         <v>16</v>
       </c>
       <c r="N9" t="s">
+        <v>105</v>
+      </c>
+      <c r="O9">
+        <v>8</v>
+      </c>
+      <c r="P9" t="s">
         <v>107</v>
-      </c>
-      <c r="O9">
-        <v>8</v>
-      </c>
-      <c r="P9" t="s">
-        <v>109</v>
       </c>
       <c r="Q9">
         <v>5</v>
@@ -1865,70 +2002,82 @@
       <c r="S9" t="s">
         <v>8</v>
       </c>
-      <c r="T9">
+      <c r="T9" t="s">
+        <v>8</v>
+      </c>
+      <c r="U9" t="s">
+        <v>8</v>
+      </c>
+      <c r="V9">
         <v>32768</v>
       </c>
-      <c r="U9" t="s">
+      <c r="W9" t="s">
+        <v>8</v>
+      </c>
+      <c r="X9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y9" t="s">
         <v>35</v>
       </c>
-      <c r="V9" s="1">
+      <c r="Z9" s="1">
         <v>125</v>
       </c>
-      <c r="W9">
+      <c r="AA9">
         <v>1169</v>
       </c>
-      <c r="X9">
+      <c r="AB9">
         <v>414</v>
       </c>
-      <c r="Y9" s="1">
+      <c r="AC9" s="1">
         <v>64</v>
       </c>
-      <c r="Z9">
+      <c r="AD9">
         <v>928</v>
       </c>
-      <c r="AA9">
+      <c r="AE9">
         <v>304</v>
       </c>
-      <c r="AB9" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC9" s="1">
+      <c r="AF9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG9" s="1">
         <v>24</v>
       </c>
-      <c r="AD9">
+      <c r="AH9">
         <v>120</v>
       </c>
-      <c r="AE9">
+      <c r="AI9">
         <v>40</v>
       </c>
-      <c r="AF9" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG9" s="1" t="s">
+      <c r="AJ9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AL9" t="s">
         <v>31</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AM9" t="s">
         <v>32</v>
       </c>
-      <c r="AJ9" s="3" t="s">
+      <c r="AN9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1937,7 +2086,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H10">
         <v>5</v>
@@ -1958,13 +2107,13 @@
         <v>16</v>
       </c>
       <c r="N10" t="s">
+        <v>105</v>
+      </c>
+      <c r="O10">
+        <v>8</v>
+      </c>
+      <c r="P10" t="s">
         <v>107</v>
-      </c>
-      <c r="O10">
-        <v>8</v>
-      </c>
-      <c r="P10" t="s">
-        <v>109</v>
       </c>
       <c r="Q10">
         <v>5</v>
@@ -1975,70 +2124,82 @@
       <c r="S10" t="s">
         <v>8</v>
       </c>
-      <c r="T10">
+      <c r="T10" t="s">
+        <v>8</v>
+      </c>
+      <c r="U10" t="s">
+        <v>8</v>
+      </c>
+      <c r="V10">
         <v>32768</v>
       </c>
-      <c r="U10" t="s">
+      <c r="W10" t="s">
+        <v>8</v>
+      </c>
+      <c r="X10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y10" t="s">
         <v>35</v>
       </c>
-      <c r="V10" s="1">
+      <c r="Z10" s="1">
         <v>125</v>
       </c>
-      <c r="W10">
+      <c r="AA10">
         <v>1169</v>
       </c>
-      <c r="X10">
+      <c r="AB10">
         <v>414</v>
       </c>
-      <c r="Y10" s="1">
+      <c r="AC10" s="1">
         <v>64</v>
       </c>
-      <c r="Z10">
+      <c r="AD10">
         <v>400</v>
       </c>
-      <c r="AA10">
+      <c r="AE10">
         <v>160</v>
       </c>
-      <c r="AB10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC10" s="1">
+      <c r="AF10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG10" s="1">
         <v>24</v>
       </c>
-      <c r="AD10">
+      <c r="AH10">
         <v>376</v>
       </c>
-      <c r="AE10">
+      <c r="AI10">
         <v>120</v>
       </c>
-      <c r="AF10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG10" s="1" t="s">
+      <c r="AJ10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AH10" t="s">
+      <c r="AL10" t="s">
         <v>31</v>
       </c>
-      <c r="AI10" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ10" t="s">
+      <c r="AM10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2047,7 +2208,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H11">
         <v>5</v>
@@ -2068,14 +2229,14 @@
         <v>16</v>
       </c>
       <c r="N11" t="s">
+        <v>105</v>
+      </c>
+      <c r="O11">
+        <v>8</v>
+      </c>
+      <c r="P11" t="s">
         <v>107</v>
       </c>
-      <c r="O11">
-        <v>8</v>
-      </c>
-      <c r="P11" t="s">
-        <v>109</v>
-      </c>
       <c r="Q11">
         <v>5</v>
       </c>
@@ -2085,70 +2246,82 @@
       <c r="S11" t="s">
         <v>8</v>
       </c>
-      <c r="T11">
+      <c r="T11" t="s">
+        <v>8</v>
+      </c>
+      <c r="U11" t="s">
+        <v>8</v>
+      </c>
+      <c r="V11">
         <v>32768</v>
       </c>
-      <c r="U11" t="s">
+      <c r="W11" t="s">
+        <v>8</v>
+      </c>
+      <c r="X11" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y11" t="s">
         <v>35</v>
       </c>
-      <c r="V11" s="1">
+      <c r="Z11" s="1">
         <v>125</v>
       </c>
-      <c r="W11">
+      <c r="AA11">
         <v>1169</v>
       </c>
-      <c r="X11">
+      <c r="AB11">
         <v>414</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="AC11" s="1">
         <v>72</v>
       </c>
-      <c r="Z11">
+      <c r="AD11">
         <v>408</v>
       </c>
-      <c r="AA11">
+      <c r="AE11">
         <v>168</v>
       </c>
-      <c r="AB11" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC11" s="1">
+      <c r="AF11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG11" s="1">
         <v>24</v>
       </c>
-      <c r="AD11">
+      <c r="AH11">
         <v>376</v>
       </c>
-      <c r="AE11">
+      <c r="AI11">
         <v>120</v>
       </c>
-      <c r="AF11" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG11" s="1" t="s">
+      <c r="AJ11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AH11" t="s">
+      <c r="AL11" t="s">
         <v>31</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AM11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="AJ11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" t="s">
-        <v>45</v>
-      </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2157,7 +2330,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H12">
         <v>5</v>
@@ -2178,14 +2351,14 @@
         <v>16</v>
       </c>
       <c r="N12" t="s">
+        <v>105</v>
+      </c>
+      <c r="O12">
+        <v>8</v>
+      </c>
+      <c r="P12" t="s">
         <v>107</v>
       </c>
-      <c r="O12">
-        <v>8</v>
-      </c>
-      <c r="P12" t="s">
-        <v>109</v>
-      </c>
       <c r="Q12">
         <v>5</v>
       </c>
@@ -2195,70 +2368,82 @@
       <c r="S12" t="s">
         <v>8</v>
       </c>
-      <c r="T12">
+      <c r="T12" t="s">
+        <v>8</v>
+      </c>
+      <c r="U12" t="s">
+        <v>8</v>
+      </c>
+      <c r="V12">
         <v>32768</v>
       </c>
-      <c r="U12" t="s">
+      <c r="W12" t="s">
+        <v>8</v>
+      </c>
+      <c r="X12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y12" t="s">
         <v>35</v>
       </c>
-      <c r="V12" s="1">
+      <c r="Z12" s="1">
         <v>125</v>
       </c>
-      <c r="W12">
+      <c r="AA12">
         <v>1169</v>
       </c>
-      <c r="X12">
+      <c r="AB12">
         <v>414</v>
       </c>
-      <c r="Y12" s="1">
+      <c r="AC12" s="1">
         <v>72</v>
       </c>
-      <c r="Z12">
+      <c r="AD12">
         <v>408</v>
       </c>
-      <c r="AA12">
+      <c r="AE12">
         <v>168</v>
       </c>
-      <c r="AB12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC12" s="1">
+      <c r="AF12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG12" s="1">
         <v>16</v>
       </c>
-      <c r="AD12">
+      <c r="AH12">
         <v>368</v>
       </c>
-      <c r="AE12">
+      <c r="AI12">
         <v>112</v>
       </c>
-      <c r="AF12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG12" s="1" t="s">
+      <c r="AJ12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AH12" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ12" t="s">
+      <c r="AL12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -2267,7 +2452,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H13">
         <v>5</v>
@@ -2288,13 +2473,13 @@
         <v>16</v>
       </c>
       <c r="N13" t="s">
+        <v>105</v>
+      </c>
+      <c r="O13">
+        <v>8</v>
+      </c>
+      <c r="P13" t="s">
         <v>107</v>
-      </c>
-      <c r="O13">
-        <v>8</v>
-      </c>
-      <c r="P13" t="s">
-        <v>109</v>
       </c>
       <c r="Q13">
         <v>5</v>
@@ -2305,70 +2490,82 @@
       <c r="S13" t="s">
         <v>8</v>
       </c>
-      <c r="T13">
+      <c r="T13" t="s">
+        <v>8</v>
+      </c>
+      <c r="U13" t="s">
+        <v>8</v>
+      </c>
+      <c r="V13">
         <v>32768</v>
       </c>
-      <c r="U13" t="s">
+      <c r="W13" t="s">
+        <v>8</v>
+      </c>
+      <c r="X13" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y13" t="s">
         <v>35</v>
       </c>
-      <c r="V13" s="1">
+      <c r="Z13" s="1">
         <v>125</v>
       </c>
-      <c r="W13">
+      <c r="AA13">
         <v>1169</v>
       </c>
-      <c r="X13">
+      <c r="AB13">
         <v>414</v>
       </c>
-      <c r="Y13" s="1">
+      <c r="AC13" s="1">
         <v>80</v>
       </c>
-      <c r="Z13">
+      <c r="AD13">
         <v>416</v>
       </c>
-      <c r="AA13">
+      <c r="AE13">
         <v>176</v>
       </c>
-      <c r="AB13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC13" s="1">
-        <v>8</v>
-      </c>
-      <c r="AD13">
+      <c r="AF13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG13" s="1">
+        <v>8</v>
+      </c>
+      <c r="AH13">
         <v>376</v>
       </c>
-      <c r="AE13">
+      <c r="AI13">
         <v>104</v>
       </c>
-      <c r="AF13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG13" s="1" t="s">
+      <c r="AJ13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AH13" t="s">
+      <c r="AL13" t="s">
         <v>31</v>
       </c>
-      <c r="AI13" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ13" t="s">
+      <c r="AM13" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2377,7 +2574,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H14">
         <v>5</v>
@@ -2398,13 +2595,13 @@
         <v>16</v>
       </c>
       <c r="N14" t="s">
+        <v>105</v>
+      </c>
+      <c r="O14">
+        <v>8</v>
+      </c>
+      <c r="P14" t="s">
         <v>107</v>
-      </c>
-      <c r="O14">
-        <v>8</v>
-      </c>
-      <c r="P14" t="s">
-        <v>109</v>
       </c>
       <c r="Q14">
         <v>5</v>
@@ -2415,70 +2612,82 @@
       <c r="S14" t="s">
         <v>8</v>
       </c>
-      <c r="T14">
+      <c r="T14" t="s">
+        <v>8</v>
+      </c>
+      <c r="U14" t="s">
+        <v>8</v>
+      </c>
+      <c r="V14">
         <v>32768</v>
       </c>
-      <c r="U14" t="s">
+      <c r="W14" t="s">
+        <v>8</v>
+      </c>
+      <c r="X14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y14" t="s">
         <v>35</v>
       </c>
-      <c r="V14" s="1">
+      <c r="Z14" s="1">
         <v>125</v>
       </c>
-      <c r="W14">
+      <c r="AA14">
         <v>1169</v>
       </c>
-      <c r="X14">
+      <c r="AB14">
         <v>414</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="AC14" s="1">
         <v>80</v>
       </c>
-      <c r="Z14">
+      <c r="AD14">
         <v>416</v>
       </c>
-      <c r="AA14">
+      <c r="AE14">
         <v>176</v>
       </c>
-      <c r="AB14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC14" s="1">
+      <c r="AF14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG14" s="1">
         <v>16</v>
       </c>
-      <c r="AD14">
+      <c r="AH14">
         <v>368</v>
       </c>
-      <c r="AE14">
+      <c r="AI14">
         <v>112</v>
       </c>
-      <c r="AF14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI14" t="s">
-        <v>8</v>
-      </c>
       <c r="AJ14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E15" s="4">
         <v>0</v>
@@ -2487,7 +2696,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H15" s="4">
         <v>5</v>
@@ -2508,13 +2717,13 @@
         <v>16</v>
       </c>
       <c r="N15" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="O15" s="4">
+        <v>8</v>
+      </c>
+      <c r="P15" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="O15" s="4">
-        <v>8</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="Q15" s="10">
         <v>10</v>
@@ -2525,70 +2734,82 @@
       <c r="S15" t="s">
         <v>8</v>
       </c>
-      <c r="T15" s="4">
+      <c r="T15" t="s">
+        <v>8</v>
+      </c>
+      <c r="U15" t="s">
+        <v>8</v>
+      </c>
+      <c r="V15" s="4">
         <v>32768</v>
       </c>
-      <c r="U15" s="4" t="s">
+      <c r="W15" t="s">
+        <v>8</v>
+      </c>
+      <c r="X15" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="V15" s="5">
+      <c r="Z15" s="5">
         <v>125</v>
       </c>
-      <c r="W15" s="4">
+      <c r="AA15" s="4">
         <v>1169</v>
       </c>
-      <c r="X15" s="4">
+      <c r="AB15" s="4">
         <v>414</v>
       </c>
-      <c r="Y15" s="5">
+      <c r="AC15" s="5">
         <v>64</v>
       </c>
-      <c r="Z15" s="4">
+      <c r="AD15" s="4">
         <v>400</v>
       </c>
-      <c r="AA15" s="4">
+      <c r="AE15" s="4">
         <v>160</v>
       </c>
-      <c r="AB15" s="4" t="s">
+      <c r="AF15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG15" s="9">
+        <v>8</v>
+      </c>
+      <c r="AH15" s="4">
+        <v>368</v>
+      </c>
+      <c r="AI15" s="4">
+        <v>96</v>
+      </c>
+      <c r="AJ15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>53</v>
       </c>
-      <c r="AC15" s="9">
-        <v>8</v>
-      </c>
-      <c r="AD15" s="4">
-        <v>368</v>
-      </c>
-      <c r="AE15" s="4">
-        <v>96</v>
-      </c>
-      <c r="AF15" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG15" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH15" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ15" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>55</v>
-      </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -2597,7 +2818,7 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H16">
         <v>5</v>
@@ -2618,13 +2839,13 @@
         <v>16</v>
       </c>
       <c r="N16" t="s">
+        <v>105</v>
+      </c>
+      <c r="O16">
+        <v>8</v>
+      </c>
+      <c r="P16" t="s">
         <v>107</v>
-      </c>
-      <c r="O16">
-        <v>8</v>
-      </c>
-      <c r="P16" t="s">
-        <v>109</v>
       </c>
       <c r="Q16">
         <v>5</v>
@@ -2635,70 +2856,82 @@
       <c r="S16" t="s">
         <v>8</v>
       </c>
-      <c r="T16">
+      <c r="T16" t="s">
+        <v>8</v>
+      </c>
+      <c r="U16" t="s">
+        <v>8</v>
+      </c>
+      <c r="V16">
         <v>32768</v>
       </c>
-      <c r="U16" t="s">
+      <c r="W16" t="s">
+        <v>8</v>
+      </c>
+      <c r="X16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y16" t="s">
         <v>35</v>
       </c>
-      <c r="V16" s="1">
+      <c r="Z16" s="1">
         <v>125</v>
       </c>
-      <c r="W16">
+      <c r="AA16">
         <v>1169</v>
       </c>
-      <c r="X16">
+      <c r="AB16">
         <v>414</v>
       </c>
-      <c r="Y16" s="1">
+      <c r="AC16" s="1">
         <v>64</v>
       </c>
-      <c r="Z16">
+      <c r="AD16">
         <v>400</v>
       </c>
-      <c r="AA16">
+      <c r="AE16">
         <v>160</v>
       </c>
-      <c r="AB16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC16" s="1">
+      <c r="AF16" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG16" s="1">
         <v>24</v>
       </c>
-      <c r="AD16">
+      <c r="AH16">
         <v>384</v>
       </c>
-      <c r="AE16">
+      <c r="AI16">
         <v>120</v>
       </c>
-      <c r="AF16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI16" t="s">
-        <v>8</v>
-      </c>
       <c r="AJ16" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2707,7 +2940,7 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H17">
         <v>5</v>
@@ -2728,13 +2961,13 @@
         <v>16</v>
       </c>
       <c r="N17" t="s">
+        <v>105</v>
+      </c>
+      <c r="O17">
+        <v>8</v>
+      </c>
+      <c r="P17" t="s">
         <v>107</v>
-      </c>
-      <c r="O17">
-        <v>8</v>
-      </c>
-      <c r="P17" t="s">
-        <v>109</v>
       </c>
       <c r="Q17">
         <v>5</v>
@@ -2745,70 +2978,82 @@
       <c r="S17" t="s">
         <v>8</v>
       </c>
-      <c r="T17">
+      <c r="T17" t="s">
+        <v>8</v>
+      </c>
+      <c r="U17" t="s">
+        <v>8</v>
+      </c>
+      <c r="V17">
         <v>32768</v>
       </c>
-      <c r="U17" t="s">
+      <c r="W17" t="s">
+        <v>8</v>
+      </c>
+      <c r="X17" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y17" t="s">
         <v>35</v>
       </c>
-      <c r="V17" s="1">
+      <c r="Z17" s="1">
         <v>125</v>
       </c>
-      <c r="W17">
+      <c r="AA17">
         <v>1169</v>
       </c>
-      <c r="X17">
+      <c r="AB17">
         <v>414</v>
       </c>
-      <c r="Y17" s="1">
+      <c r="AC17" s="1">
         <v>64</v>
       </c>
-      <c r="Z17">
+      <c r="AD17">
         <v>400</v>
       </c>
-      <c r="AA17">
+      <c r="AE17">
         <v>176</v>
       </c>
-      <c r="AB17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC17" s="1">
+      <c r="AF17" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG17" s="1">
         <v>24</v>
       </c>
-      <c r="AD17">
+      <c r="AH17">
         <v>384</v>
       </c>
-      <c r="AE17">
+      <c r="AI17">
         <v>112</v>
       </c>
-      <c r="AF17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>8</v>
-      </c>
       <c r="AJ17" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2817,7 +3062,7 @@
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H18">
         <v>5</v>
@@ -2838,13 +3083,13 @@
         <v>16</v>
       </c>
       <c r="N18" t="s">
+        <v>105</v>
+      </c>
+      <c r="O18">
+        <v>8</v>
+      </c>
+      <c r="P18" t="s">
         <v>107</v>
-      </c>
-      <c r="O18">
-        <v>8</v>
-      </c>
-      <c r="P18" t="s">
-        <v>109</v>
       </c>
       <c r="Q18">
         <v>5</v>
@@ -2855,70 +3100,82 @@
       <c r="S18" t="s">
         <v>8</v>
       </c>
-      <c r="T18">
+      <c r="T18" t="s">
+        <v>8</v>
+      </c>
+      <c r="U18" t="s">
+        <v>8</v>
+      </c>
+      <c r="V18">
         <v>32768</v>
       </c>
-      <c r="U18" t="s">
+      <c r="W18" t="s">
+        <v>8</v>
+      </c>
+      <c r="X18" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y18" t="s">
         <v>35</v>
       </c>
-      <c r="V18" s="1">
+      <c r="Z18" s="1">
         <v>125</v>
       </c>
-      <c r="W18">
+      <c r="AA18">
         <v>1169</v>
       </c>
-      <c r="X18">
+      <c r="AB18">
         <v>414</v>
       </c>
-      <c r="Y18" s="1">
+      <c r="AC18" s="1">
         <v>64</v>
       </c>
-      <c r="Z18">
+      <c r="AD18">
         <v>400</v>
       </c>
-      <c r="AA18">
+      <c r="AE18">
         <v>192</v>
       </c>
-      <c r="AB18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC18" s="1">
+      <c r="AF18" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG18" s="1">
         <v>24</v>
       </c>
-      <c r="AD18">
+      <c r="AH18">
         <v>384</v>
       </c>
-      <c r="AE18">
+      <c r="AI18">
         <v>104</v>
       </c>
-      <c r="AF18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI18" t="s">
-        <v>8</v>
-      </c>
       <c r="AJ18" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -2927,7 +3184,7 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H19">
         <v>5</v>
@@ -2948,13 +3205,13 @@
         <v>16</v>
       </c>
       <c r="N19" t="s">
+        <v>105</v>
+      </c>
+      <c r="O19">
+        <v>8</v>
+      </c>
+      <c r="P19" t="s">
         <v>107</v>
-      </c>
-      <c r="O19">
-        <v>8</v>
-      </c>
-      <c r="P19" t="s">
-        <v>109</v>
       </c>
       <c r="Q19">
         <v>5</v>
@@ -2965,70 +3222,82 @@
       <c r="S19" t="s">
         <v>8</v>
       </c>
-      <c r="T19">
+      <c r="T19" t="s">
+        <v>8</v>
+      </c>
+      <c r="U19" t="s">
+        <v>8</v>
+      </c>
+      <c r="V19">
         <v>32768</v>
       </c>
-      <c r="U19" t="s">
+      <c r="W19" t="s">
+        <v>8</v>
+      </c>
+      <c r="X19" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y19" t="s">
         <v>35</v>
       </c>
-      <c r="V19" s="1">
+      <c r="Z19" s="1">
         <v>125</v>
       </c>
-      <c r="W19">
+      <c r="AA19">
         <v>1169</v>
       </c>
-      <c r="X19">
+      <c r="AB19">
         <v>414</v>
       </c>
-      <c r="Y19" s="1">
+      <c r="AC19" s="1">
         <v>64</v>
       </c>
-      <c r="Z19">
+      <c r="AD19">
         <v>416</v>
       </c>
-      <c r="AA19">
+      <c r="AE19">
         <v>160</v>
       </c>
-      <c r="AB19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC19" s="1">
+      <c r="AF19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG19" s="1">
         <v>24</v>
       </c>
-      <c r="AD19">
+      <c r="AH19">
         <v>376</v>
       </c>
-      <c r="AE19">
+      <c r="AI19">
         <v>120</v>
       </c>
-      <c r="AF19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI19" t="s">
-        <v>8</v>
-      </c>
       <c r="AJ19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -3037,7 +3306,7 @@
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H20">
         <v>5</v>
@@ -3058,13 +3327,13 @@
         <v>16</v>
       </c>
       <c r="N20" t="s">
+        <v>105</v>
+      </c>
+      <c r="O20">
+        <v>8</v>
+      </c>
+      <c r="P20" t="s">
         <v>107</v>
-      </c>
-      <c r="O20">
-        <v>8</v>
-      </c>
-      <c r="P20" t="s">
-        <v>109</v>
       </c>
       <c r="Q20">
         <v>5</v>
@@ -3075,70 +3344,82 @@
       <c r="S20" t="s">
         <v>8</v>
       </c>
-      <c r="T20">
+      <c r="T20" t="s">
+        <v>8</v>
+      </c>
+      <c r="U20" t="s">
+        <v>8</v>
+      </c>
+      <c r="V20">
         <v>32768</v>
       </c>
-      <c r="U20" t="s">
+      <c r="W20" t="s">
+        <v>8</v>
+      </c>
+      <c r="X20" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y20" t="s">
         <v>35</v>
       </c>
-      <c r="V20" s="1">
+      <c r="Z20" s="1">
         <v>125</v>
       </c>
-      <c r="W20">
+      <c r="AA20">
         <v>1169</v>
       </c>
-      <c r="X20">
+      <c r="AB20">
         <v>414</v>
       </c>
-      <c r="Y20" s="1">
+      <c r="AC20" s="1">
         <v>64</v>
       </c>
-      <c r="Z20">
+      <c r="AD20">
         <v>432</v>
       </c>
-      <c r="AA20">
+      <c r="AE20">
         <v>160</v>
       </c>
-      <c r="AB20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC20" s="1">
+      <c r="AF20" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG20" s="1">
         <v>24</v>
       </c>
-      <c r="AD20">
+      <c r="AH20">
         <v>368</v>
       </c>
-      <c r="AE20">
+      <c r="AI20">
         <v>120</v>
       </c>
-      <c r="AF20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG20" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI20" t="s">
-        <v>8</v>
-      </c>
       <c r="AJ20" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -3147,7 +3428,7 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H21">
         <v>5</v>
@@ -3168,13 +3449,13 @@
         <v>16</v>
       </c>
       <c r="N21" t="s">
+        <v>105</v>
+      </c>
+      <c r="O21">
+        <v>8</v>
+      </c>
+      <c r="P21" t="s">
         <v>107</v>
-      </c>
-      <c r="O21">
-        <v>8</v>
-      </c>
-      <c r="P21" t="s">
-        <v>109</v>
       </c>
       <c r="Q21">
         <v>5</v>
@@ -3185,70 +3466,82 @@
       <c r="S21" t="s">
         <v>8</v>
       </c>
-      <c r="T21">
+      <c r="T21" t="s">
+        <v>8</v>
+      </c>
+      <c r="U21" t="s">
+        <v>8</v>
+      </c>
+      <c r="V21">
         <v>32768</v>
       </c>
-      <c r="U21" t="s">
+      <c r="W21" t="s">
+        <v>8</v>
+      </c>
+      <c r="X21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y21" t="s">
         <v>35</v>
       </c>
-      <c r="V21" s="1">
+      <c r="Z21" s="1">
         <v>125</v>
       </c>
-      <c r="W21">
+      <c r="AA21">
         <v>1169</v>
       </c>
-      <c r="X21">
+      <c r="AB21">
         <v>414</v>
       </c>
-      <c r="Y21" s="1">
+      <c r="AC21" s="1">
         <v>80</v>
       </c>
-      <c r="Z21">
+      <c r="AD21">
         <v>400</v>
       </c>
-      <c r="AA21">
+      <c r="AE21">
         <v>160</v>
       </c>
-      <c r="AB21" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC21" s="1">
+      <c r="AF21" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG21" s="1">
         <v>16</v>
       </c>
-      <c r="AD21">
+      <c r="AH21">
         <v>384</v>
       </c>
-      <c r="AE21">
+      <c r="AI21">
         <v>120</v>
       </c>
-      <c r="AF21" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG21" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH21" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI21" t="s">
-        <v>8</v>
-      </c>
       <c r="AJ21" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -3257,7 +3550,7 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H22">
         <v>5</v>
@@ -3278,13 +3571,13 @@
         <v>16</v>
       </c>
       <c r="N22" t="s">
+        <v>105</v>
+      </c>
+      <c r="O22">
+        <v>8</v>
+      </c>
+      <c r="P22" t="s">
         <v>107</v>
-      </c>
-      <c r="O22">
-        <v>8</v>
-      </c>
-      <c r="P22" t="s">
-        <v>109</v>
       </c>
       <c r="Q22">
         <v>5</v>
@@ -3295,508 +3588,635 @@
       <c r="S22" t="s">
         <v>8</v>
       </c>
-      <c r="T22">
+      <c r="T22" t="s">
+        <v>8</v>
+      </c>
+      <c r="U22" t="s">
+        <v>8</v>
+      </c>
+      <c r="V22">
         <v>32768</v>
       </c>
-      <c r="U22" t="s">
+      <c r="W22" t="s">
+        <v>8</v>
+      </c>
+      <c r="X22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y22" t="s">
         <v>35</v>
       </c>
-      <c r="V22" s="1">
+      <c r="Z22" s="1">
         <v>125</v>
       </c>
-      <c r="W22">
+      <c r="AA22">
         <v>1169</v>
       </c>
-      <c r="X22">
+      <c r="AB22">
         <v>414</v>
       </c>
-      <c r="Y22" s="1">
+      <c r="AC22" s="1">
         <v>96</v>
       </c>
-      <c r="Z22">
+      <c r="AD22">
         <v>400</v>
       </c>
-      <c r="AA22">
+      <c r="AE22">
         <v>160</v>
       </c>
-      <c r="AB22" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC22" s="1">
-        <v>8</v>
-      </c>
-      <c r="AD22">
+      <c r="AF22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG22" s="1">
+        <v>8</v>
+      </c>
+      <c r="AH22">
         <v>384</v>
       </c>
-      <c r="AE22">
+      <c r="AI22">
         <v>120</v>
       </c>
-      <c r="AF22" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG22" s="1" t="s">
+      <c r="AJ22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M23" t="s">
+        <v>8</v>
+      </c>
+      <c r="N23" t="s">
+        <v>8</v>
+      </c>
+      <c r="O23" t="s">
+        <v>8</v>
+      </c>
+      <c r="P23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>8</v>
+      </c>
+      <c r="R23" t="s">
+        <v>8</v>
+      </c>
+      <c r="S23" t="s">
+        <v>8</v>
+      </c>
+      <c r="T23" t="s">
+        <v>8</v>
+      </c>
+      <c r="U23" t="s">
+        <v>8</v>
+      </c>
+      <c r="V23" t="s">
+        <v>8</v>
+      </c>
+      <c r="W23" t="s">
+        <v>8</v>
+      </c>
+      <c r="X23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="AH22" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI22" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ22" t="s">
+      <c r="D24" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="R24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="S24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="T24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="U24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="V24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="W24" t="s">
+        <v>8</v>
+      </c>
+      <c r="X24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z24" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC24" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG24" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK24" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN24" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" t="s">
         <v>113</v>
       </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D23" t="s">
-        <v>117</v>
-      </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" t="s">
-        <v>8</v>
-      </c>
-      <c r="I23" t="s">
-        <v>8</v>
-      </c>
-      <c r="J23" t="s">
-        <v>8</v>
-      </c>
-      <c r="K23" t="s">
-        <v>8</v>
-      </c>
-      <c r="L23" t="s">
-        <v>8</v>
-      </c>
-      <c r="M23" t="s">
-        <v>8</v>
-      </c>
-      <c r="N23" t="s">
-        <v>8</v>
-      </c>
-      <c r="O23" t="s">
-        <v>8</v>
-      </c>
-      <c r="P23" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>8</v>
-      </c>
-      <c r="R23" t="s">
-        <v>8</v>
-      </c>
-      <c r="S23" t="s">
-        <v>8</v>
-      </c>
-      <c r="T23" t="s">
-        <v>8</v>
-      </c>
-      <c r="U23" t="s">
-        <v>8</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="W23" t="s">
-        <v>8</v>
-      </c>
-      <c r="X23" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="13" t="s">
+      <c r="C25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25" s="16">
+        <v>0</v>
+      </c>
+      <c r="F25" s="16">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="K24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="L24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="M24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="N24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="O24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="P24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="R24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="S24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="T24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="U24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="V24" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="W24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="X24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y24" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC24" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG24" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ24" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:36" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="H25" s="15">
-        <v>5</v>
-      </c>
-      <c r="I25" s="15">
-        <v>3</v>
-      </c>
-      <c r="J25" s="15">
+      <c r="H25">
+        <v>5</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="J25">
         <v>2</v>
       </c>
-      <c r="K25" s="15">
-        <v>3</v>
-      </c>
-      <c r="L25" s="15">
+      <c r="K25">
+        <v>3</v>
+      </c>
+      <c r="L25">
         <v>1</v>
       </c>
       <c r="M25">
         <v>16</v>
       </c>
       <c r="N25" t="s">
+        <v>105</v>
+      </c>
+      <c r="O25">
+        <v>8</v>
+      </c>
+      <c r="P25" t="s">
         <v>107</v>
       </c>
-      <c r="O25">
-        <v>8</v>
-      </c>
-      <c r="P25" t="s">
-        <v>109</v>
-      </c>
-      <c r="S25" s="14">
-        <f t="shared" ref="S25" si="0" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (Y25*Z25*AA25)</f>
+      <c r="Q25" s="16">
+        <v>5</v>
+      </c>
+      <c r="R25" t="s">
+        <v>124</v>
+      </c>
+      <c r="S25" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="T25" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="U25">
+        <f t="shared" ref="U25" si="0" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AC25*AD25*AE25)</f>
         <v>83027.753778838392</v>
       </c>
-      <c r="T25" s="14">
+      <c r="V25">
         <v>81920</v>
       </c>
-      <c r="U25" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="V25" s="1">
+      <c r="W25">
+        <v>81049.600000000006</v>
+      </c>
+      <c r="X25">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z25" s="1">
         <v>125</v>
       </c>
-      <c r="W25" s="14">
+      <c r="AA25">
         <v>1169</v>
       </c>
-      <c r="X25" s="14">
+      <c r="AB25">
         <v>414</v>
       </c>
-      <c r="Y25" s="1">
+      <c r="AC25" s="1">
         <v>112</v>
       </c>
-      <c r="Z25" s="14">
+      <c r="AD25">
         <v>864</v>
       </c>
-      <c r="AA25" s="14">
+      <c r="AE25">
         <v>400</v>
       </c>
-      <c r="AB25" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC25" s="1">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((V25 - Y25) / 2)</f>
+      <c r="AF25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG25" s="1">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((Z25 - AC25) / 2)</f>
         <v>6</v>
       </c>
-      <c r="AD25" s="14">
-        <f t="shared" ref="AD25" si="1" xml:space="preserve"> _xlfn.FLOOR.MATH((W25 - Z25) / 2)</f>
+      <c r="AH25">
+        <f t="shared" ref="AH25" si="1" xml:space="preserve"> _xlfn.FLOOR.MATH((AA25 - AD25) / 2)</f>
         <v>152</v>
       </c>
-      <c r="AE25" s="14">
-        <f t="shared" ref="AE25" si="2" xml:space="preserve"> _xlfn.FLOOR.MATH((X25 - AA25) / 2)</f>
+      <c r="AI25">
+        <f t="shared" ref="AI25" si="2" xml:space="preserve"> _xlfn.FLOOR.MATH((AB25 - AE25) / 2)</f>
         <v>7</v>
       </c>
-      <c r="AF25" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH25" t="s">
-        <v>125</v>
+      <c r="AJ25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL25" t="s">
+        <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B26" s="15" t="s">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" t="s">
         <v>121</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="H26" s="15">
-        <v>5</v>
-      </c>
-      <c r="I26" s="15">
-        <v>3</v>
-      </c>
-      <c r="J26" s="15">
+      <c r="D26" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26" s="16">
+        <v>0</v>
+      </c>
+      <c r="F26" s="16">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>76</v>
+      </c>
+      <c r="H26">
+        <v>5</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
         <v>2</v>
       </c>
-      <c r="K26" s="15">
-        <v>3</v>
-      </c>
-      <c r="L26" s="15">
+      <c r="K26">
+        <v>3</v>
+      </c>
+      <c r="L26">
         <v>1</v>
       </c>
       <c r="M26">
         <v>16</v>
       </c>
       <c r="N26" t="s">
+        <v>105</v>
+      </c>
+      <c r="O26">
+        <v>8</v>
+      </c>
+      <c r="P26" t="s">
         <v>107</v>
       </c>
-      <c r="O26">
-        <v>8</v>
-      </c>
-      <c r="P26" t="s">
-        <v>109</v>
-      </c>
-      <c r="S26" s="14">
-        <f t="shared" ref="S26" si="3" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (Y26*Z26*AA26)</f>
+      <c r="Q26" s="16">
+        <v>5</v>
+      </c>
+      <c r="R26" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="S26" s="16">
+        <v>82032.639999999999</v>
+      </c>
+      <c r="T26" s="16">
+        <f xml:space="preserve"> 75.58 + 4.53</f>
+        <v>80.11</v>
+      </c>
+      <c r="U26">
+        <f t="shared" ref="U26:U27" si="3" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AC26*AD26*AE26)</f>
         <v>81518.129922434266</v>
       </c>
-      <c r="T26" s="14">
+      <c r="V26">
         <v>81920</v>
       </c>
-      <c r="U26" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="V26" s="1">
+      <c r="W26">
+        <v>81049.600000000006</v>
+      </c>
+      <c r="X26">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z26" s="1">
         <v>125</v>
       </c>
-      <c r="W26" s="14">
+      <c r="AA26">
         <v>1169</v>
       </c>
-      <c r="X26" s="14">
+      <c r="AB26">
         <v>414</v>
       </c>
-      <c r="Y26" s="1">
+      <c r="AC26" s="1">
         <v>112</v>
       </c>
-      <c r="Z26" s="14">
+      <c r="AD26">
         <v>848</v>
       </c>
-      <c r="AA26" s="14">
+      <c r="AE26">
         <v>400</v>
       </c>
-      <c r="AB26" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC26" s="1">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((V26 - Y26) / 2)</f>
+      <c r="AF26" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG26" s="1">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((Z26 - AC26) / 2)</f>
         <v>6</v>
       </c>
-      <c r="AD26" s="14">
-        <f t="shared" ref="AD26" si="4" xml:space="preserve"> _xlfn.FLOOR.MATH((W26 - Z26) / 2)</f>
+      <c r="AH26">
+        <f t="shared" ref="AH26" si="4" xml:space="preserve"> _xlfn.FLOOR.MATH((AA26 - AD26) / 2)</f>
         <v>160</v>
       </c>
-      <c r="AE26" s="14">
-        <f t="shared" ref="AE26" si="5" xml:space="preserve"> _xlfn.FLOOR.MATH((X26 - AA26) / 2)</f>
+      <c r="AI26">
+        <f t="shared" ref="AI26" si="5" xml:space="preserve"> _xlfn.FLOOR.MATH((AB26 - AE26) / 2)</f>
         <v>7</v>
       </c>
-      <c r="AF26" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH26" t="s">
+      <c r="AJ26" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL26" t="s">
+        <v>123</v>
+      </c>
+      <c r="AM26" t="s">
         <v>125</v>
       </c>
+      <c r="AN26" t="s">
+        <v>126</v>
+      </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="14"/>
-      <c r="W28" s="14"/>
-      <c r="X28" s="14"/>
-      <c r="Z28" s="14"/>
-      <c r="AA28" s="14"/>
-      <c r="AB28" s="14"/>
-      <c r="AD28" s="14"/>
-      <c r="AE28" s="14"/>
-      <c r="AF28" s="14"/>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="Z29" s="14"/>
-      <c r="AA29" s="14"/>
-    </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="Z30" s="14"/>
-      <c r="AA30" s="14"/>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="Z31" s="14"/>
-      <c r="AA31" s="14"/>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="Z32" s="14"/>
-      <c r="AA32" s="14"/>
-    </row>
-    <row r="33" spans="26:27" x14ac:dyDescent="0.25">
-      <c r="Z33" s="14"/>
-      <c r="AA33" s="14"/>
-    </row>
-    <row r="34" spans="26:27" x14ac:dyDescent="0.25">
-      <c r="Z34" s="14"/>
-      <c r="AA34" s="14"/>
-    </row>
-    <row r="35" spans="26:27" x14ac:dyDescent="0.25">
-      <c r="Z35" s="14"/>
-      <c r="AA35" s="14"/>
-    </row>
-    <row r="36" spans="26:27" x14ac:dyDescent="0.25">
-      <c r="Z36" s="14"/>
-      <c r="AA36" s="14"/>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q27" s="16">
+        <v>5</v>
+      </c>
+      <c r="R27">
+        <v>77887</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="3"/>
+        <v>76989.258353221856</v>
+      </c>
+      <c r="V27">
+        <v>81920</v>
+      </c>
+      <c r="W27">
+        <v>81049.600000000006</v>
+      </c>
+      <c r="X27">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>125</v>
+      </c>
+      <c r="AA27">
+        <v>1169</v>
+      </c>
+      <c r="AB27">
+        <v>414</v>
+      </c>
+      <c r="AC27" s="1">
+        <v>112</v>
+      </c>
+      <c r="AD27">
+        <v>800</v>
+      </c>
+      <c r="AE27">
+        <v>400</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG27" s="1">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((Z27 - AC27) / 2)</f>
+        <v>6</v>
+      </c>
+      <c r="AH27">
+        <f t="shared" ref="AH27" si="6" xml:space="preserve"> _xlfn.FLOOR.MATH((AA27 - AD27) / 2)</f>
+        <v>184</v>
+      </c>
+      <c r="AI27">
+        <f t="shared" ref="AI27" si="7" xml:space="preserve"> _xlfn.FLOOR.MATH((AB27 - AE27) / 2)</f>
+        <v>7</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK27" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>134</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>